<commit_message>
review 2nd round - 1st question
</commit_message>
<xml_diff>
--- a/data/tuning_and_performance.xlsx
+++ b/data/tuning_and_performance.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LENKA\STU\PHD\Science\self tunable HE\repository\self_tunable_HE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B7EE50-E491-4CFA-95D5-FDAA569A25C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF63A546-AC66-4A6D-9F2D-6C8960EF9940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FDE36F7A-3726-4B54-89C5-B98D2615A837}"/>
+    <workbookView xWindow="-2660" yWindow="1270" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FDE36F7A-3726-4B54-89C5-B98D2615A837}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
     <sheet name="Hárok2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="85">
   <si>
     <r>
       <t>Q</t>
@@ -658,7 +657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -755,14 +754,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
@@ -774,7 +765,10 @@
     <xf numFmtId="9" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -1092,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24187AA2-D870-438E-B038-0C0C3317218D}">
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1628,14 +1622,8 @@
       </c>
       <c r="G31" s="28"/>
     </row>
-    <row r="32" spans="1:7" s="89" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="86"/>
-      <c r="B32" s="88"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="86"/>
-      <c r="G32" s="86"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B32" s="32"/>
     </row>
     <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="7" t="s">
@@ -1661,15 +1649,15 @@
       <c r="B35" s="9">
         <v>1000</v>
       </c>
-      <c r="C35" s="99">
+      <c r="C35" s="93">
         <f>(C16-$C$19)/$C$19</f>
         <v>5.3097345132743362E-2</v>
       </c>
-      <c r="D35" s="99">
+      <c r="D35" s="93">
         <f>(D16-$D$19)/$D$19</f>
         <v>1.2053982883475971</v>
       </c>
-      <c r="E35" s="99">
+      <c r="E35" s="93">
         <f>(F16-$F$19)/$F$19</f>
         <v>0.73684210526315785</v>
       </c>
@@ -1679,33 +1667,33 @@
       <c r="B36" s="2">
         <v>100</v>
       </c>
-      <c r="C36" s="99">
+      <c r="C36" s="93">
         <f>(C17-$C$19)/$C$19</f>
         <v>0.27876106194690264</v>
       </c>
-      <c r="D36" s="99">
+      <c r="D36" s="93">
         <f>(D17-$D$19)/$D$19</f>
         <v>9.6115865701119171E-2</v>
       </c>
-      <c r="E36" s="99">
+      <c r="E36" s="93">
         <f>(F17-$F$19)/$F$19</f>
         <v>0.31578947368421051</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="94"/>
-      <c r="B37" s="95">
+      <c r="A37" s="88"/>
+      <c r="B37" s="89">
         <v>500</v>
       </c>
-      <c r="C37" s="99">
+      <c r="C37" s="93">
         <f>(C18-$C$19)/$C$19</f>
         <v>-0.14011799410029499</v>
       </c>
-      <c r="D37" s="100">
+      <c r="D37" s="94">
         <f>(D18-$D$19)/$D$19</f>
         <v>0.15536537195523359</v>
       </c>
-      <c r="E37" s="99">
+      <c r="E37" s="93">
         <f>(F18-$F$19)/$F$19</f>
         <v>-0.21052631578947367</v>
       </c>
@@ -1717,15 +1705,15 @@
       <c r="B38" s="21">
         <v>1000</v>
       </c>
-      <c r="C38" s="101">
+      <c r="C38" s="95">
         <f>(C20-$C$23)/$C$23</f>
         <v>0.47177419354838712</v>
       </c>
-      <c r="D38" s="101">
+      <c r="D38" s="95">
         <f>(D20-$D$23)/$D$23</f>
         <v>1.467328802927339</v>
       </c>
-      <c r="E38" s="101">
+      <c r="E38" s="95">
         <f>(F20-$F$23)/$F$23</f>
         <v>-0.47368421052631576</v>
       </c>
@@ -1735,33 +1723,33 @@
       <c r="B39" s="3">
         <v>100</v>
       </c>
-      <c r="C39" s="101">
+      <c r="C39" s="95">
         <f>(C21-$C$23)/$C$23</f>
         <v>1.4435483870967742</v>
       </c>
-      <c r="D39" s="101">
+      <c r="D39" s="95">
         <f>(D21-$D$23)/$D$23</f>
         <v>0.21536853110297968</v>
       </c>
-      <c r="E39" s="101">
+      <c r="E39" s="95">
         <f>(F21-$F$23)/$F$23</f>
         <v>1.7894736842105263</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="96"/>
-      <c r="B40" s="97">
+      <c r="A40" s="90"/>
+      <c r="B40" s="91">
         <v>500</v>
       </c>
-      <c r="C40" s="101">
+      <c r="C40" s="95">
         <f>(C22-$C$23)/$C$23</f>
         <v>-0.32258064516129031</v>
       </c>
-      <c r="D40" s="101">
+      <c r="D40" s="95">
         <f>(D22-$D$23)/$D$23</f>
         <v>-4.9660219550444376E-2</v>
       </c>
-      <c r="E40" s="101">
+      <c r="E40" s="95">
         <f>(F22-$F$23)/$F$23</f>
         <v>-0.31578947368421051</v>
       </c>
@@ -1773,15 +1761,15 @@
       <c r="B41" s="9">
         <v>1000</v>
       </c>
-      <c r="C41" s="99">
+      <c r="C41" s="93">
         <f>(C24-$C$27)/$C$27</f>
         <v>0.31720430107526881</v>
       </c>
-      <c r="D41" s="99">
+      <c r="D41" s="93">
         <f>(D24-$D$27)/$D$27</f>
         <v>-0.23058153721024807</v>
       </c>
-      <c r="E41" s="99">
+      <c r="E41" s="93">
         <f>(F24-$F$27)/$F$27</f>
         <v>0</v>
       </c>
@@ -1791,33 +1779,33 @@
       <c r="B42" s="2">
         <v>100</v>
       </c>
-      <c r="C42" s="99">
+      <c r="C42" s="93">
         <f>(C25-$C$27)/$C$27</f>
         <v>1.1397849462365592</v>
       </c>
-      <c r="D42" s="99">
+      <c r="D42" s="93">
         <f>(D25-$D$27)/$D$27</f>
         <v>2.2387149247661648</v>
       </c>
-      <c r="E42" s="99">
+      <c r="E42" s="93">
         <f>(F25-$F$27)/$F$27</f>
         <v>3.7692307692307692</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="94"/>
-      <c r="B43" s="95">
+      <c r="A43" s="88"/>
+      <c r="B43" s="89">
         <v>500</v>
       </c>
-      <c r="C43" s="100">
+      <c r="C43" s="94">
         <f>(C26-$C$27)/$C$27</f>
         <v>0.13440860215053763</v>
       </c>
-      <c r="D43" s="99">
+      <c r="D43" s="93">
         <f>(D26-$D$27)/$D$27</f>
         <v>-9.2313948759658385E-2</v>
       </c>
-      <c r="E43" s="100">
+      <c r="E43" s="94">
         <f>(F26-$F$27)/$F$27</f>
         <v>0.23076923076923078</v>
       </c>
@@ -1829,15 +1817,15 @@
       <c r="B44" s="21">
         <v>1000</v>
       </c>
-      <c r="C44" s="101">
+      <c r="C44" s="95">
         <f>(C28-$C$31)/$C$31</f>
         <v>5.894519131334023E-2</v>
       </c>
-      <c r="D44" s="101">
+      <c r="D44" s="95">
         <f>(D28-$D$31)/$D$31</f>
         <v>0.11764705882352942</v>
       </c>
-      <c r="E44" s="101">
+      <c r="E44" s="95">
         <f>(F28-$F$31)/$F$31</f>
         <v>0.21621621621621623</v>
       </c>
@@ -1847,39 +1835,36 @@
       <c r="B45" s="3">
         <v>100</v>
       </c>
-      <c r="C45" s="101">
+      <c r="C45" s="95">
         <f>(C29-$C$31)/$C$31</f>
         <v>0.4498448810754912</v>
       </c>
-      <c r="D45" s="101">
+      <c r="D45" s="95">
         <f>(D29-$D$31)/$D$31</f>
         <v>1.5391146149181325</v>
       </c>
-      <c r="E45" s="101">
+      <c r="E45" s="95">
         <f>(F29-$F$31)/$F$31</f>
         <v>3.8648648648648649</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="98"/>
+      <c r="A46" s="92"/>
       <c r="B46" s="1">
         <v>500</v>
       </c>
-      <c r="C46" s="102">
+      <c r="C46" s="96">
         <f>(C30-$C$31)/$C$31</f>
         <v>0.10031023784901758</v>
       </c>
-      <c r="D46" s="102">
+      <c r="D46" s="96">
         <f>(D30-$D$31)/$D$31</f>
         <v>0.55427531837477251</v>
       </c>
-      <c r="E46" s="102">
+      <c r="E46" s="96">
         <f>(F30-$F$31)/$F$31</f>
         <v>2.6216216216216215</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="90"/>
     </row>
     <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="7" t="s">
@@ -1944,15 +1929,15 @@
         <v>1000</v>
       </c>
       <c r="C51" s="62">
-        <f>C38*100</f>
+        <f t="shared" ref="C51:E52" si="1">C38*100</f>
         <v>47.177419354838712</v>
       </c>
       <c r="D51" s="62">
-        <f>D38*100</f>
+        <f t="shared" si="1"/>
         <v>146.73288029273391</v>
       </c>
       <c r="E51" s="62">
-        <f>E38*100</f>
+        <f t="shared" si="1"/>
         <v>-47.368421052631575</v>
       </c>
     </row>
@@ -1962,15 +1947,15 @@
         <v>100</v>
       </c>
       <c r="C52" s="62">
-        <f>C39*100</f>
+        <f t="shared" si="1"/>
         <v>144.35483870967744</v>
       </c>
       <c r="D52" s="62">
-        <f>D39*100</f>
+        <f t="shared" si="1"/>
         <v>21.536853110297969</v>
       </c>
       <c r="E52" s="62">
-        <f>E39*100</f>
+        <f t="shared" si="1"/>
         <v>178.94736842105263</v>
       </c>
     </row>
@@ -1982,15 +1967,15 @@
         <v>1000</v>
       </c>
       <c r="C53" s="59">
-        <f>C41*100</f>
+        <f t="shared" ref="C53:E54" si="2">C41*100</f>
         <v>31.72043010752688</v>
       </c>
       <c r="D53" s="59">
-        <f>D41*100</f>
+        <f t="shared" si="2"/>
         <v>-23.058153721024809</v>
       </c>
       <c r="E53" s="59">
-        <f>E41*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2000,15 +1985,15 @@
         <v>100</v>
       </c>
       <c r="C54" s="59">
-        <f>C42*100</f>
+        <f t="shared" si="2"/>
         <v>113.97849462365592</v>
       </c>
       <c r="D54" s="59">
-        <f>D42*100</f>
+        <f t="shared" si="2"/>
         <v>223.87149247661648</v>
       </c>
       <c r="E54" s="59">
-        <f>E42*100</f>
+        <f t="shared" si="2"/>
         <v>376.92307692307691</v>
       </c>
     </row>
@@ -2020,15 +2005,15 @@
         <v>1000</v>
       </c>
       <c r="C55" s="62">
-        <f t="shared" ref="C55:E56" si="1">C44*100</f>
+        <f t="shared" ref="C55:E56" si="3">C44*100</f>
         <v>5.8945191313340226</v>
       </c>
       <c r="D55" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.764705882352942</v>
       </c>
       <c r="E55" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>21.621621621621621</v>
       </c>
     </row>
@@ -2038,23 +2023,19 @@
         <v>100</v>
       </c>
       <c r="C56" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44.984488107549119</v>
       </c>
       <c r="D56" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>153.91146149181324</v>
       </c>
       <c r="E56" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>386.48648648648651</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="90"/>
-    </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="90"/>
       <c r="B58" t="s">
         <v>84</v>
       </c>
@@ -2082,97 +2063,80 @@
         <v>1000</v>
       </c>
       <c r="C60" s="62">
-        <f>AVERAGE(C49,C51,C53,C55)</f>
+        <f t="shared" ref="C60:E61" si="4">AVERAGE(C49,C51,C53,C55)</f>
         <v>22.525525776743486</v>
       </c>
       <c r="D60" s="62">
-        <f>AVERAGE(D49,D51,D53,D55)</f>
+        <f t="shared" si="4"/>
         <v>63.99481532220544</v>
       </c>
       <c r="E60" s="62">
-        <f>AVERAGE(E49,E51,E53,E55)</f>
+        <f t="shared" si="4"/>
         <v>11.984352773826457</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="80"/>
-      <c r="B61" s="92">
-        <v>100</v>
-      </c>
-      <c r="C61" s="93">
-        <f>AVERAGE(C50,C52,C54,C56)</f>
+      <c r="B61" s="86">
+        <v>100</v>
+      </c>
+      <c r="C61" s="87">
+        <f t="shared" si="4"/>
         <v>82.79848190889318</v>
       </c>
-      <c r="D61" s="93">
-        <f>AVERAGE(D50,D52,D54,D56)</f>
+      <c r="D61" s="87">
+        <f t="shared" si="4"/>
         <v>102.2328484122099</v>
       </c>
-      <c r="E61" s="93">
-        <f>AVERAGE(E50,E52,E54,E56)</f>
+      <c r="E61" s="87">
+        <f t="shared" si="4"/>
         <v>243.48396979975928</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="89" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="87"/>
-      <c r="B62" s="103">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="1"/>
+      <c r="B62" s="37">
         <v>500</v>
       </c>
-      <c r="C62" s="93">
+      <c r="C62" s="87">
         <f>AVERAGE(C37,C40,C43,C46)</f>
         <v>-5.6994949815507519E-2</v>
       </c>
-      <c r="D62" s="93">
+      <c r="D62" s="87">
         <f>AVERAGE(D37,D40,D43,D46)</f>
         <v>0.14191663050497583</v>
       </c>
-      <c r="E62" s="93">
+      <c r="E62" s="87">
         <f>AVERAGE(E37,E40,E43,E46)</f>
         <v>0.58151876572929206</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="89" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="86"/>
-      <c r="B63" s="86"/>
-      <c r="C63" s="91"/>
-      <c r="D63" s="91"/>
-      <c r="E63" s="91"/>
-    </row>
-    <row r="64" spans="1:5" s="89" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="86"/>
-      <c r="B64" s="86"/>
-      <c r="C64" s="91"/>
-      <c r="D64" s="91"/>
-      <c r="E64" s="91"/>
-    </row>
-    <row r="65" spans="1:7" s="89" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="86"/>
-      <c r="B65" s="86"/>
-      <c r="C65" s="91"/>
-      <c r="D65" s="91"/>
-      <c r="E65" s="91"/>
-    </row>
-    <row r="66" spans="1:7" s="89" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="86"/>
-      <c r="B66" s="86"/>
-      <c r="C66" s="91"/>
-      <c r="D66" s="91"/>
-      <c r="E66" s="91"/>
-    </row>
-    <row r="67" spans="1:7" s="89" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="86"/>
-      <c r="B67" s="86"/>
-      <c r="C67" s="91"/>
-      <c r="D67" s="91"/>
-      <c r="E67" s="91"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="86"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" s="86"/>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C63" s="76"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="76"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C64" s="76"/>
+      <c r="D64" s="76"/>
+      <c r="E64" s="76"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C65" s="76"/>
+      <c r="D65" s="76"/>
+      <c r="E65" s="76"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C66" s="76"/>
+      <c r="D66" s="76"/>
+      <c r="E66" s="76"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C67" s="76"/>
+      <c r="D67" s="76"/>
+      <c r="E67" s="76"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="86"/>
       <c r="B70">
         <v>28</v>
       </c>
@@ -2975,8 +2939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCC6C2E-BC1D-47B4-A935-B6D151C5A89E}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="D31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3217,7 +3181,7 @@
       <c r="M15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N15" s="7" t="s">
+      <c r="N15" s="39" t="s">
         <v>25</v>
       </c>
       <c r="O15" s="7" t="s">
@@ -3257,7 +3221,7 @@
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
-      <c r="N16" s="10"/>
+      <c r="N16" s="41"/>
       <c r="O16" s="11"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
@@ -3289,7 +3253,7 @@
       <c r="K17" s="13"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
+      <c r="N17" s="45"/>
       <c r="O17" s="4"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3327,7 +3291,7 @@
         <f>(MIN(E16:E17)-E18)/MIN(E16:E17)</f>
         <v>8.7687687687687699E-2</v>
       </c>
-      <c r="N18" s="61">
+      <c r="N18" s="97">
         <f>(MIN(G16:G17)-G18)/MIN(G16:G17)</f>
         <v>-0.12264150943396215</v>
       </c>
@@ -3369,7 +3333,7 @@
       </c>
       <c r="L19" s="17"/>
       <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
+      <c r="N19" s="50"/>
       <c r="O19" s="17"/>
     </row>
     <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3401,7 +3365,7 @@
       <c r="K20" s="23"/>
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
+      <c r="N20" s="50"/>
       <c r="O20" s="17"/>
     </row>
     <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3439,7 +3403,7 @@
         <f>(MIN(E19:E20)-E21)/MIN(E19:E20)</f>
         <v>0.17720430107526888</v>
       </c>
-      <c r="N21" s="61">
+      <c r="N21" s="97">
         <f t="shared" ref="N21:N27" si="0">(MIN(G19:G20)-G21)/MIN(G19:G20)</f>
         <v>-0.34538152610441758</v>
       </c>
@@ -3481,7 +3445,7 @@
       </c>
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
+      <c r="N22" s="50"/>
       <c r="O22" s="17"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3513,7 +3477,7 @@
       <c r="K23" s="13"/>
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
+      <c r="N23" s="50"/>
       <c r="O23" s="17"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3551,7 +3515,7 @@
         <f>(MIN(E22:E23)-E24)/MIN(E22:E23)</f>
         <v>-0.29968287526427062</v>
       </c>
-      <c r="N24" s="61">
+      <c r="N24" s="97">
         <f t="shared" si="0"/>
         <v>-4.4776119402985232E-2</v>
       </c>
@@ -3593,7 +3557,7 @@
       </c>
       <c r="L25" s="17"/>
       <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
+      <c r="N25" s="50"/>
       <c r="O25" s="17"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3625,7 +3589,7 @@
       <c r="K26" s="23"/>
       <c r="L26" s="17"/>
       <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
+      <c r="N26" s="50"/>
       <c r="O26" s="17"/>
     </row>
     <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3663,7 +3627,7 @@
         <f>(MIN(E25:E26)-E27)/MIN(E25:E26)</f>
         <v>0.10526315789473685</v>
       </c>
-      <c r="N27" s="17">
+      <c r="N27" s="50">
         <f t="shared" si="0"/>
         <v>-0.18279569892473121</v>
       </c>
@@ -3677,14 +3641,14 @@
         <v>79</v>
       </c>
       <c r="L28" s="76">
-        <f t="shared" ref="L28:M28" si="2">AVERAGE(L18,L21,L24,L27)</f>
+        <f>AVERAGE(L18,L21,L24,L27)</f>
         <v>0.16686212557582963</v>
       </c>
       <c r="M28" s="76">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="L28:M28" si="2">AVERAGE(M18,M21,M24,M27)</f>
         <v>1.761806784835571E-2</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="38">
         <f>AVERAGE(N18,N21,N24,N27)</f>
         <v>-0.17389871346652405</v>
       </c>
@@ -3693,7 +3657,7 @@
         <v>-0.12055555555555555</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="38"/>
       <c r="B30" s="38">
         <v>28</v>
@@ -3703,6 +3667,18 @@
       <c r="E30" s="38"/>
       <c r="F30" s="38"/>
       <c r="G30" s="38"/>
+      <c r="K30" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="39" t="s">
@@ -3726,8 +3702,23 @@
       <c r="G31" s="39" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="K31" s="8">
+        <v>1</v>
+      </c>
+      <c r="L31" s="93">
+        <f>(C16-$C$18)/C16</f>
+        <v>5.0420168067226892E-2</v>
+      </c>
+      <c r="M31" s="93">
+        <f>(E16-$E$18)/E16</f>
+        <v>0.54656716417910445</v>
+      </c>
+      <c r="N31" s="93">
+        <f>(I16-$I$18)/I16</f>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="40">
         <v>1</v>
       </c>
@@ -3747,8 +3738,21 @@
         <v>45062</v>
       </c>
       <c r="G32" s="43"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K32" s="13"/>
+      <c r="L32" s="93">
+        <f>(C17-$C$18)/C17</f>
+        <v>0.2179930795847751</v>
+      </c>
+      <c r="M32" s="93">
+        <f>(E17-$E$18)/E17</f>
+        <v>8.7687687687687699E-2</v>
+      </c>
+      <c r="N32" s="93">
+        <f>(I17-$I$18)/I17</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="44"/>
       <c r="B33" s="45">
         <v>100</v>
@@ -3766,8 +3770,12 @@
         <v>45058</v>
       </c>
       <c r="G33" s="47"/>
-    </row>
-    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K33" s="15"/>
+      <c r="L33" s="93"/>
+      <c r="M33" s="93"/>
+      <c r="N33" s="93"/>
+    </row>
+    <row r="34" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="48"/>
       <c r="B34" s="49" t="s">
         <v>15</v>
@@ -3785,8 +3793,23 @@
         <v>45057</v>
       </c>
       <c r="G34" s="52"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K34" s="20">
+        <v>2</v>
+      </c>
+      <c r="L34" s="95">
+        <f>(C19-$C$21)/C19</f>
+        <v>0.32054794520547947</v>
+      </c>
+      <c r="M34" s="95">
+        <f>(E19-$E$21)/E19</f>
+        <v>0.59470338983050841</v>
+      </c>
+      <c r="N34" s="95">
+        <f>(I19-$I$21)/I19</f>
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="40">
         <v>2</v>
       </c>
@@ -3806,8 +3829,21 @@
         <v>5</v>
       </c>
       <c r="G35" s="53"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K35" s="23"/>
+      <c r="L35" s="95">
+        <f>(C20-$C$21)/C20</f>
+        <v>0.5907590759075908</v>
+      </c>
+      <c r="M35" s="95">
+        <f>(E20-$E$21)/E20</f>
+        <v>0.17720430107526888</v>
+      </c>
+      <c r="N35" s="95">
+        <f>(I20-$I$21)/I20</f>
+        <v>0.64150943396226412</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="44"/>
       <c r="B36" s="45">
         <v>100</v>
@@ -3825,8 +3861,12 @@
         <v>45072</v>
       </c>
       <c r="G36" s="47"/>
-    </row>
-    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K36" s="25"/>
+      <c r="L36" s="95"/>
+      <c r="M36" s="99"/>
+      <c r="N36" s="95"/>
+    </row>
+    <row r="37" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="48"/>
       <c r="B37" s="49" t="s">
         <v>15</v>
@@ -3844,8 +3884,23 @@
         <v>17</v>
       </c>
       <c r="G37" s="52"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K37" s="8">
+        <v>3</v>
+      </c>
+      <c r="L37" s="93">
+        <f>(C22-$C$24)/C22</f>
+        <v>0.24081632653061225</v>
+      </c>
+      <c r="M37" s="93">
+        <f>(E22-$E$24)/E22</f>
+        <v>-0.29968287526427062</v>
+      </c>
+      <c r="N37" s="93">
+        <f>(I22-$I$24)/I22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="40">
         <v>3</v>
       </c>
@@ -3865,8 +3920,21 @@
         <v>45052</v>
       </c>
       <c r="G38" s="43"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K38" s="13"/>
+      <c r="L38" s="93">
+        <f>(C23-$C$24)/C23</f>
+        <v>0.53266331658291455</v>
+      </c>
+      <c r="M38" s="93">
+        <f>(E23-$E$24)/E23</f>
+        <v>0.69123556002009034</v>
+      </c>
+      <c r="N38" s="93">
+        <f>(I23-$I$24)/I23</f>
+        <v>0.79032258064516125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="44"/>
       <c r="B39" s="45">
         <v>100</v>
@@ -3884,8 +3952,12 @@
         <v>31</v>
       </c>
       <c r="G39" s="47"/>
-    </row>
-    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K39" s="15"/>
+      <c r="L39" s="93"/>
+      <c r="M39" s="93"/>
+      <c r="N39" s="93"/>
+    </row>
+    <row r="40" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="48"/>
       <c r="B40" s="49" t="s">
         <v>15</v>
@@ -3903,8 +3975,23 @@
         <v>45052</v>
       </c>
       <c r="G40" s="52"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K40" s="20">
+        <v>4</v>
+      </c>
+      <c r="L40" s="95">
+        <f>(C25-$C$27)/C25</f>
+        <v>5.56640625E-2</v>
+      </c>
+      <c r="M40" s="95">
+        <f>(E25-$E$27)/E25</f>
+        <v>0.10526315789473685</v>
+      </c>
+      <c r="N40" s="95">
+        <f>(I25-$I$27)/I25</f>
+        <v>0.17777777777777778</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" s="40">
         <v>4</v>
       </c>
@@ -3924,8 +4011,21 @@
         <v>45068</v>
       </c>
       <c r="G41" s="53"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K41" s="23"/>
+      <c r="L41" s="95">
+        <f>(C26-$C$27)/C26</f>
+        <v>0.3102710413694722</v>
+      </c>
+      <c r="M41" s="95">
+        <f>(E26-$E$27)/E26</f>
+        <v>0.6061619297826607</v>
+      </c>
+      <c r="N41" s="95">
+        <f>(I26-$I$27)/I26</f>
+        <v>0.7944444444444444</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="44"/>
       <c r="B42" s="45">
         <v>100</v>
@@ -3943,8 +4043,12 @@
         <v>90</v>
       </c>
       <c r="G42" s="47"/>
-    </row>
-    <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K42" s="25"/>
+      <c r="L42" s="98"/>
+      <c r="M42" s="98"/>
+      <c r="N42" s="98"/>
+    </row>
+    <row r="43" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="48"/>
       <c r="B43" s="49" t="s">
         <v>15</v>
@@ -3962,8 +4066,38 @@
         <v>45063</v>
       </c>
       <c r="G43" s="52"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K43" t="s">
+        <v>79</v>
+      </c>
+      <c r="L43" s="100">
+        <f>AVERAGE(L31,L34,L37,L40)</f>
+        <v>0.16686212557582963</v>
+      </c>
+      <c r="M43" s="100">
+        <f>AVERAGE(M31,M34,M37,M40)</f>
+        <v>0.23671270916001977</v>
+      </c>
+      <c r="N43" s="100">
+        <f>AVERAGE(N31,N34,N37,N40)</f>
+        <v>-7.4494949494949503E-2</v>
+      </c>
+      <c r="O43" s="76"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L44" s="100">
+        <f>AVERAGE(L32,L35,L38,L41)</f>
+        <v>0.41292162836118818</v>
+      </c>
+      <c r="M44" s="100">
+        <f>AVERAGE(M32,M35,M38,M41)</f>
+        <v>0.39057236964142694</v>
+      </c>
+      <c r="N44" s="100">
+        <f>AVERAGE(N32,N35,N38,N41)</f>
+        <v>0.61656911476296739</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="38"/>
       <c r="B46" s="38">
         <v>29</v>
@@ -3974,7 +4108,7 @@
       <c r="F46" s="38"/>
       <c r="G46" s="38"/>
     </row>
-    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="39" t="s">
         <v>19</v>
       </c>
@@ -3997,7 +4131,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" s="40">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
review 2nd round - 2nd question
</commit_message>
<xml_diff>
--- a/data/tuning_and_performance.xlsx
+++ b/data/tuning_and_performance.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LENKA\STU\PHD\Science\self tunable HE\repository\self_tunable_HE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF63A546-AC66-4A6D-9F2D-6C8960EF9940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8997672B-23C4-43FB-A1BA-43D4566AD65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2660" yWindow="1270" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FDE36F7A-3726-4B54-89C5-B98D2615A837}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{FDE36F7A-3726-4B54-89C5-B98D2615A837}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
     <sheet name="Hárok2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hárok3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="85">
   <si>
     <r>
       <t>Q</t>
@@ -376,7 +377,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,6 +420,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -657,7 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -769,6 +776,11 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -1087,7 +1099,7 @@
   <dimension ref="A1:G118"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="A15" sqref="A15:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2939,8 +2951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCC6C2E-BC1D-47B4-A935-B6D151C5A89E}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3645,7 +3657,7 @@
         <v>0.16686212557582963</v>
       </c>
       <c r="M28" s="76">
-        <f t="shared" ref="L28:M28" si="2">AVERAGE(M18,M21,M24,M27)</f>
+        <f t="shared" ref="M28" si="2">AVERAGE(M18,M21,M24,M27)</f>
         <v>1.761806784835571E-2</v>
       </c>
       <c r="N28" s="38">
@@ -4070,30 +4082,30 @@
         <v>79</v>
       </c>
       <c r="L43" s="100">
-        <f>AVERAGE(L31,L34,L37,L40)</f>
+        <f t="shared" ref="L43:N44" si="3">AVERAGE(L31,L34,L37,L40)</f>
         <v>0.16686212557582963</v>
       </c>
       <c r="M43" s="100">
-        <f>AVERAGE(M31,M34,M37,M40)</f>
+        <f t="shared" si="3"/>
         <v>0.23671270916001977</v>
       </c>
       <c r="N43" s="100">
-        <f>AVERAGE(N31,N34,N37,N40)</f>
+        <f t="shared" si="3"/>
         <v>-7.4494949494949503E-2</v>
       </c>
       <c r="O43" s="76"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="L44" s="100">
-        <f>AVERAGE(L32,L35,L38,L41)</f>
+        <f t="shared" si="3"/>
         <v>0.41292162836118818</v>
       </c>
       <c r="M44" s="100">
-        <f>AVERAGE(M32,M35,M38,M41)</f>
+        <f t="shared" si="3"/>
         <v>0.39057236964142694</v>
       </c>
       <c r="N44" s="100">
-        <f>AVERAGE(N32,N35,N38,N41)</f>
+        <f t="shared" si="3"/>
         <v>0.61656911476296739</v>
       </c>
     </row>
@@ -4370,4 +4382,585 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C35220-4847-41A4-99D4-689044B6F5A0}">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="9.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="9">
+        <v>714</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="E2" s="9">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="13"/>
+      <c r="B3" s="2">
+        <v>100</v>
+      </c>
+      <c r="C3" s="2">
+        <v>867</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.16650000000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="77"/>
+      <c r="B4" s="78">
+        <v>500</v>
+      </c>
+      <c r="C4" s="84">
+        <v>583</v>
+      </c>
+      <c r="D4" s="78">
+        <v>0.17549999999999999</v>
+      </c>
+      <c r="E4" s="84">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="15"/>
+      <c r="B5" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="17">
+        <v>678</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0.15190000000000001</v>
+      </c>
+      <c r="E5" s="17">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="20">
+        <v>2</v>
+      </c>
+      <c r="B6" s="21">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="21">
+        <v>365</v>
+      </c>
+      <c r="D6" s="21">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="E6" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="23"/>
+      <c r="B7" s="3">
+        <v>100</v>
+      </c>
+      <c r="C7" s="3">
+        <v>606</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.23250000000000001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="80"/>
+      <c r="B8" s="81">
+        <v>500</v>
+      </c>
+      <c r="C8" s="84">
+        <v>168</v>
+      </c>
+      <c r="D8" s="84">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="E8" s="84">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="25"/>
+      <c r="B9" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="17">
+        <v>248</v>
+      </c>
+      <c r="D9" s="17">
+        <v>0.1913</v>
+      </c>
+      <c r="E9" s="26">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
+        <v>3</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C10" s="9">
+        <v>245</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.18920000000000001</v>
+      </c>
+      <c r="E10" s="9">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="13"/>
+      <c r="B11" s="2">
+        <v>100</v>
+      </c>
+      <c r="C11" s="2">
+        <v>398</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.7964</v>
+      </c>
+      <c r="E11" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="77"/>
+      <c r="B12" s="78">
+        <v>500</v>
+      </c>
+      <c r="C12" s="78">
+        <v>211</v>
+      </c>
+      <c r="D12" s="84">
+        <v>0.22320000000000001</v>
+      </c>
+      <c r="E12" s="78">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="15"/>
+      <c r="B13" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="17">
+        <v>186</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0.24590000000000001</v>
+      </c>
+      <c r="E13" s="17">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="20">
+        <v>4</v>
+      </c>
+      <c r="B14" s="21">
+        <v>1000</v>
+      </c>
+      <c r="C14" s="21">
+        <v>1024</v>
+      </c>
+      <c r="D14" s="21">
+        <v>0.18429999999999999</v>
+      </c>
+      <c r="E14" s="21">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="23"/>
+      <c r="B15" s="3">
+        <v>100</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1402</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.41870000000000002</v>
+      </c>
+      <c r="E15" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="80"/>
+      <c r="B16" s="81">
+        <v>500</v>
+      </c>
+      <c r="C16" s="81">
+        <v>1064</v>
+      </c>
+      <c r="D16" s="81">
+        <v>0.25629999999999997</v>
+      </c>
+      <c r="E16" s="81">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="25"/>
+      <c r="B17" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="17">
+        <v>967</v>
+      </c>
+      <c r="D17" s="17">
+        <v>0.16489999999999999</v>
+      </c>
+      <c r="E17" s="17">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="8">
+        <v>1</v>
+      </c>
+      <c r="B21" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C21" s="93">
+        <f>(C2-$C$5)/C2</f>
+        <v>5.0420168067226892E-2</v>
+      </c>
+      <c r="D21" s="93">
+        <f>(D2-$D$5)/D2</f>
+        <v>0.54656716417910445</v>
+      </c>
+      <c r="E21" s="93">
+        <f>(E2-$E$5)/E2</f>
+        <v>0.42424242424242425</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="13"/>
+      <c r="B22" s="2">
+        <v>100</v>
+      </c>
+      <c r="C22" s="93">
+        <f t="shared" ref="C22:C26" si="0">(C3-$C$5)/C3</f>
+        <v>0.2179930795847751</v>
+      </c>
+      <c r="D22" s="93">
+        <f t="shared" ref="D22:D23" si="1">(D3-$D$5)/D3</f>
+        <v>8.7687687687687699E-2</v>
+      </c>
+      <c r="E22" s="93">
+        <f t="shared" ref="E22:E23" si="2">(E3-$E$5)/E3</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="15"/>
+      <c r="B23" s="78">
+        <v>500</v>
+      </c>
+      <c r="C23" s="93">
+        <f>(C4-$C$5)/C4</f>
+        <v>-0.16295025728987994</v>
+      </c>
+      <c r="D23" s="93">
+        <f t="shared" si="1"/>
+        <v>0.13447293447293437</v>
+      </c>
+      <c r="E23" s="93">
+        <f t="shared" si="2"/>
+        <v>-0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="20">
+        <v>2</v>
+      </c>
+      <c r="B24" s="21">
+        <v>1000</v>
+      </c>
+      <c r="C24" s="95">
+        <f>(C6-$C$9)/C6</f>
+        <v>0.32054794520547947</v>
+      </c>
+      <c r="D24" s="95">
+        <f>(D6-$D$9)/D6</f>
+        <v>0.59470338983050841</v>
+      </c>
+      <c r="E24" s="95">
+        <f>(E6-$E$9)/E6</f>
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="23"/>
+      <c r="B25" s="3">
+        <v>100</v>
+      </c>
+      <c r="C25" s="95">
+        <f t="shared" ref="C25:C27" si="3">(C7-$C$9)/C7</f>
+        <v>0.5907590759075908</v>
+      </c>
+      <c r="D25" s="95">
+        <f t="shared" ref="D25:D26" si="4">(D7-$D$9)/D7</f>
+        <v>0.17720430107526888</v>
+      </c>
+      <c r="E25" s="95">
+        <f t="shared" ref="E25:E26" si="5">(E7-$E$9)/E7</f>
+        <v>0.64150943396226412</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="25"/>
+      <c r="B26" s="81">
+        <v>500</v>
+      </c>
+      <c r="C26" s="95">
+        <f t="shared" si="3"/>
+        <v>-0.47619047619047616</v>
+      </c>
+      <c r="D26" s="95">
+        <f t="shared" si="4"/>
+        <v>-5.2255225522552302E-2</v>
+      </c>
+      <c r="E26" s="95">
+        <f t="shared" si="5"/>
+        <v>-0.46153846153846156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="8">
+        <v>3</v>
+      </c>
+      <c r="B27" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C27" s="93">
+        <f>(C10-$C$13)/C10</f>
+        <v>0.24081632653061225</v>
+      </c>
+      <c r="D27" s="93">
+        <f>(D10-$D$13)/D10</f>
+        <v>-0.29968287526427062</v>
+      </c>
+      <c r="E27" s="93">
+        <f>(E10-$E$13)/E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="13"/>
+      <c r="B28" s="2">
+        <v>100</v>
+      </c>
+      <c r="C28" s="93">
+        <f t="shared" ref="C28:C30" si="6">(C11-$C$13)/C11</f>
+        <v>0.53266331658291455</v>
+      </c>
+      <c r="D28" s="93">
+        <f t="shared" ref="D28:D29" si="7">(D11-$D$13)/D11</f>
+        <v>0.69123556002009034</v>
+      </c>
+      <c r="E28" s="93">
+        <f t="shared" ref="E28:E29" si="8">(E11-$E$13)/E11</f>
+        <v>0.79032258064516125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="15"/>
+      <c r="B29" s="78">
+        <v>500</v>
+      </c>
+      <c r="C29" s="93">
+        <f t="shared" si="6"/>
+        <v>0.11848341232227488</v>
+      </c>
+      <c r="D29" s="93">
+        <f t="shared" si="7"/>
+        <v>-0.10170250896057347</v>
+      </c>
+      <c r="E29" s="93">
+        <f t="shared" si="8"/>
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="20">
+        <v>4</v>
+      </c>
+      <c r="B30" s="21">
+        <v>1000</v>
+      </c>
+      <c r="C30" s="95">
+        <f>(C14-$C$17)/C14</f>
+        <v>5.56640625E-2</v>
+      </c>
+      <c r="D30" s="95">
+        <f>(D14-$D$17)/D14</f>
+        <v>0.10526315789473685</v>
+      </c>
+      <c r="E30" s="95">
+        <f>(E14-$E$17)/E14</f>
+        <v>0.17777777777777778</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="23"/>
+      <c r="B31" s="3">
+        <v>100</v>
+      </c>
+      <c r="C31" s="95">
+        <f t="shared" ref="C31:C32" si="9">(C15-$C$17)/C15</f>
+        <v>0.3102710413694722</v>
+      </c>
+      <c r="D31" s="95">
+        <f t="shared" ref="D31:D32" si="10">(D15-$D$17)/D15</f>
+        <v>0.6061619297826607</v>
+      </c>
+      <c r="E31" s="95">
+        <f t="shared" ref="E31:E32" si="11">(E15-$E$17)/E15</f>
+        <v>0.7944444444444444</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="25"/>
+      <c r="B32" s="81">
+        <v>500</v>
+      </c>
+      <c r="C32" s="95">
+        <f t="shared" si="9"/>
+        <v>9.1165413533834588E-2</v>
+      </c>
+      <c r="D32" s="95">
+        <f t="shared" si="10"/>
+        <v>0.35661334373780723</v>
+      </c>
+      <c r="E32" s="95">
+        <f t="shared" si="11"/>
+        <v>0.72388059701492535</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="104" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="101">
+        <v>1000</v>
+      </c>
+      <c r="C33" s="105">
+        <f>AVERAGE(C21,C24,C27,C30)</f>
+        <v>0.16686212557582963</v>
+      </c>
+      <c r="D33" s="105">
+        <f t="shared" ref="D33:E33" si="12">AVERAGE(D21,D24,D27,D30)</f>
+        <v>0.23671270916001977</v>
+      </c>
+      <c r="E33" s="105">
+        <f t="shared" si="12"/>
+        <v>-7.4494949494949503E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="104"/>
+      <c r="B34" s="102">
+        <v>100</v>
+      </c>
+      <c r="C34" s="105">
+        <f t="shared" ref="C34:E35" si="13">AVERAGE(C22,C25,C28,C31)</f>
+        <v>0.41292162836118818</v>
+      </c>
+      <c r="D34" s="105">
+        <f t="shared" si="13"/>
+        <v>0.39057236964142694</v>
+      </c>
+      <c r="E34" s="105">
+        <f t="shared" si="13"/>
+        <v>0.61656911476296739</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="104"/>
+      <c r="B35" s="103">
+        <v>500</v>
+      </c>
+      <c r="C35" s="105">
+        <f t="shared" si="13"/>
+        <v>-0.10737297690606165</v>
+      </c>
+      <c r="D35" s="105">
+        <f t="shared" si="13"/>
+        <v>8.4282135931903965E-2</v>
+      </c>
+      <c r="E35" s="105">
+        <f t="shared" si="13"/>
+        <v>4.5793867202449268E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
review 2nd round - 3rd question
</commit_message>
<xml_diff>
--- a/data/tuning_and_performance.xlsx
+++ b/data/tuning_and_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LENKA\STU\PHD\Science\self tunable HE\repository\self_tunable_HE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8997672B-23C4-43FB-A1BA-43D4566AD65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5730DC-CE27-4DBF-8CDC-220B61A59F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{FDE36F7A-3726-4B54-89C5-B98D2615A837}"/>
+    <workbookView xWindow="22932" yWindow="-4560" windowWidth="30936" windowHeight="16776" xr2:uid="{FDE36F7A-3726-4B54-89C5-B98D2615A837}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="85">
   <si>
     <r>
       <t>Q</t>
@@ -323,7 +323,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
@@ -660,11 +661,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -781,8 +783,12 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Čiarka" xfId="2" builtinId="3"/>
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
     <cellStyle name="Percentá" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1098,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24187AA2-D870-438E-B038-0C0C3317218D}">
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:F31"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4386,10 +4392,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C35220-4847-41A4-99D4-689044B6F5A0}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4648,7 +4654,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="25"/>
       <c r="B17" s="34" t="s">
         <v>15</v>
@@ -4663,7 +4669,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
@@ -4679,8 +4685,23 @@
       <c r="E20" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="8">
         <v>1</v>
       </c>
@@ -4699,14 +4720,32 @@
         <f>(E2-$E$5)/E2</f>
         <v>0.42424242424242425</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G21" s="8">
+        <v>1</v>
+      </c>
+      <c r="H21" s="9">
+        <v>1000</v>
+      </c>
+      <c r="I21" s="106">
+        <f>C2/$C$5</f>
+        <v>1.0530973451327434</v>
+      </c>
+      <c r="J21" s="106">
+        <f>D2/$D$5</f>
+        <v>2.2053982883475971</v>
+      </c>
+      <c r="K21" s="106">
+        <f>E2/$E$5</f>
+        <v>1.736842105263158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="13"/>
       <c r="B22" s="2">
         <v>100</v>
       </c>
       <c r="C22" s="93">
-        <f t="shared" ref="C22:C26" si="0">(C3-$C$5)/C3</f>
+        <f t="shared" ref="C22" si="0">(C3-$C$5)/C3</f>
         <v>0.2179930795847751</v>
       </c>
       <c r="D22" s="93">
@@ -4717,8 +4756,24 @@
         <f t="shared" ref="E22:E23" si="2">(E3-$E$5)/E3</f>
         <v>0.24</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G22" s="13"/>
+      <c r="H22" s="2">
+        <v>100</v>
+      </c>
+      <c r="I22" s="106">
+        <f t="shared" ref="I22" si="3">C3/$C$5</f>
+        <v>1.2787610619469028</v>
+      </c>
+      <c r="J22" s="106">
+        <f t="shared" ref="J22:J23" si="4">D3/$D$5</f>
+        <v>1.0961158657011192</v>
+      </c>
+      <c r="K22" s="106">
+        <f t="shared" ref="K22:K23" si="5">E3/$E$5</f>
+        <v>1.3157894736842106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="15"/>
       <c r="B23" s="78">
         <v>500</v>
@@ -4735,8 +4790,24 @@
         <f t="shared" si="2"/>
         <v>-0.26666666666666666</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G23" s="15"/>
+      <c r="H23" s="78">
+        <v>500</v>
+      </c>
+      <c r="I23" s="106">
+        <f>C4/$C$5</f>
+        <v>0.85988200589970498</v>
+      </c>
+      <c r="J23" s="106">
+        <f t="shared" si="4"/>
+        <v>1.1553653719552335</v>
+      </c>
+      <c r="K23" s="106">
+        <f t="shared" si="5"/>
+        <v>0.78947368421052633</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="20">
         <v>2</v>
       </c>
@@ -4755,44 +4826,94 @@
         <f>(E6-$E$9)/E6</f>
         <v>-0.9</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G24" s="20">
+        <v>2</v>
+      </c>
+      <c r="H24" s="21">
+        <v>1000</v>
+      </c>
+      <c r="I24" s="107">
+        <f>C6/$C$9</f>
+        <v>1.471774193548387</v>
+      </c>
+      <c r="J24" s="107">
+        <f>D6/$D$9</f>
+        <v>2.467328802927339</v>
+      </c>
+      <c r="K24" s="107">
+        <f>E6/$E$9</f>
+        <v>0.52631578947368418</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="23"/>
       <c r="B25" s="3">
         <v>100</v>
       </c>
       <c r="C25" s="95">
-        <f t="shared" ref="C25:C27" si="3">(C7-$C$9)/C7</f>
+        <f t="shared" ref="C25:C26" si="6">(C7-$C$9)/C7</f>
         <v>0.5907590759075908</v>
       </c>
       <c r="D25" s="95">
-        <f t="shared" ref="D25:D26" si="4">(D7-$D$9)/D7</f>
+        <f t="shared" ref="D25:D26" si="7">(D7-$D$9)/D7</f>
         <v>0.17720430107526888</v>
       </c>
       <c r="E25" s="95">
-        <f t="shared" ref="E25:E26" si="5">(E7-$E$9)/E7</f>
+        <f t="shared" ref="E25:E26" si="8">(E7-$E$9)/E7</f>
         <v>0.64150943396226412</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G25" s="23"/>
+      <c r="H25" s="3">
+        <v>100</v>
+      </c>
+      <c r="I25" s="107">
+        <f t="shared" ref="I25:I26" si="9">C7/$C$9</f>
+        <v>2.443548387096774</v>
+      </c>
+      <c r="J25" s="107">
+        <f t="shared" ref="J25:J26" si="10">D7/$D$9</f>
+        <v>1.2153685311029796</v>
+      </c>
+      <c r="K25" s="107">
+        <f t="shared" ref="K25:K26" si="11">E7/$E$9</f>
+        <v>2.7894736842105261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="25"/>
       <c r="B26" s="81">
         <v>500</v>
       </c>
       <c r="C26" s="95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-0.47619047619047616</v>
       </c>
       <c r="D26" s="95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-5.2255225522552302E-2</v>
       </c>
       <c r="E26" s="95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>-0.46153846153846156</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G26" s="25"/>
+      <c r="H26" s="81">
+        <v>500</v>
+      </c>
+      <c r="I26" s="107">
+        <f t="shared" si="9"/>
+        <v>0.67741935483870963</v>
+      </c>
+      <c r="J26" s="107">
+        <f t="shared" si="10"/>
+        <v>0.95033978044955558</v>
+      </c>
+      <c r="K26" s="107">
+        <f t="shared" si="11"/>
+        <v>0.68421052631578949</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="8">
         <v>3</v>
       </c>
@@ -4811,44 +4932,94 @@
         <f>(E10-$E$13)/E10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G27" s="8">
+        <v>3</v>
+      </c>
+      <c r="H27" s="9">
+        <v>1000</v>
+      </c>
+      <c r="I27" s="106">
+        <f>C10/$C$13</f>
+        <v>1.3172043010752688</v>
+      </c>
+      <c r="J27" s="106">
+        <f>D10/$D$13</f>
+        <v>0.7694184627897519</v>
+      </c>
+      <c r="K27" s="106">
+        <f>E10/$E$13</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="13"/>
       <c r="B28" s="2">
         <v>100</v>
       </c>
       <c r="C28" s="93">
-        <f t="shared" ref="C28:C30" si="6">(C11-$C$13)/C11</f>
+        <f t="shared" ref="C28:C29" si="12">(C11-$C$13)/C11</f>
         <v>0.53266331658291455</v>
       </c>
       <c r="D28" s="93">
-        <f t="shared" ref="D28:D29" si="7">(D11-$D$13)/D11</f>
+        <f t="shared" ref="D28:D29" si="13">(D11-$D$13)/D11</f>
         <v>0.69123556002009034</v>
       </c>
       <c r="E28" s="93">
-        <f t="shared" ref="E28:E29" si="8">(E11-$E$13)/E11</f>
+        <f t="shared" ref="E28:E29" si="14">(E11-$E$13)/E11</f>
         <v>0.79032258064516125</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G28" s="13"/>
+      <c r="H28" s="2">
+        <v>100</v>
+      </c>
+      <c r="I28" s="106">
+        <f t="shared" ref="I28:I29" si="15">C11/$C$13</f>
+        <v>2.139784946236559</v>
+      </c>
+      <c r="J28" s="106">
+        <f t="shared" ref="J28:J29" si="16">D11/$D$13</f>
+        <v>3.2387149247661648</v>
+      </c>
+      <c r="K28" s="106">
+        <f t="shared" ref="K28:K29" si="17">E11/$E$13</f>
+        <v>4.7692307692307692</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="15"/>
       <c r="B29" s="78">
         <v>500</v>
       </c>
       <c r="C29" s="93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.11848341232227488</v>
       </c>
       <c r="D29" s="93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>-0.10170250896057347</v>
       </c>
       <c r="E29" s="93">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.1875</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G29" s="15"/>
+      <c r="H29" s="78">
+        <v>500</v>
+      </c>
+      <c r="I29" s="106">
+        <f t="shared" si="15"/>
+        <v>1.1344086021505377</v>
+      </c>
+      <c r="J29" s="106">
+        <f t="shared" si="16"/>
+        <v>0.90768605124034163</v>
+      </c>
+      <c r="K29" s="106">
+        <f t="shared" si="17"/>
+        <v>1.2307692307692308</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="20">
         <v>4</v>
       </c>
@@ -4867,44 +5038,94 @@
         <f>(E14-$E$17)/E14</f>
         <v>0.17777777777777778</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G30" s="20">
+        <v>4</v>
+      </c>
+      <c r="H30" s="21">
+        <v>1000</v>
+      </c>
+      <c r="I30" s="107">
+        <f>C14/$C$17</f>
+        <v>1.0589451913133403</v>
+      </c>
+      <c r="J30" s="107">
+        <f>D14/$D$17</f>
+        <v>1.1176470588235294</v>
+      </c>
+      <c r="K30" s="107">
+        <f>E14/$E$17</f>
+        <v>1.2162162162162162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="23"/>
       <c r="B31" s="3">
         <v>100</v>
       </c>
       <c r="C31" s="95">
-        <f t="shared" ref="C31:C32" si="9">(C15-$C$17)/C15</f>
+        <f t="shared" ref="C31:C32" si="18">(C15-$C$17)/C15</f>
         <v>0.3102710413694722</v>
       </c>
       <c r="D31" s="95">
-        <f t="shared" ref="D31:D32" si="10">(D15-$D$17)/D15</f>
+        <f t="shared" ref="D31:D32" si="19">(D15-$D$17)/D15</f>
         <v>0.6061619297826607</v>
       </c>
       <c r="E31" s="95">
-        <f t="shared" ref="E31:E32" si="11">(E15-$E$17)/E15</f>
+        <f t="shared" ref="E31:E32" si="20">(E15-$E$17)/E15</f>
         <v>0.7944444444444444</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G31" s="23"/>
+      <c r="H31" s="3">
+        <v>100</v>
+      </c>
+      <c r="I31" s="107">
+        <f t="shared" ref="I31:I32" si="21">C15/$C$17</f>
+        <v>1.4498448810754911</v>
+      </c>
+      <c r="J31" s="107">
+        <f t="shared" ref="J31:J32" si="22">D15/$D$17</f>
+        <v>2.5391146149181325</v>
+      </c>
+      <c r="K31" s="107">
+        <f t="shared" ref="K31:K32" si="23">E15/$E$17</f>
+        <v>4.8648648648648649</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="25"/>
       <c r="B32" s="81">
         <v>500</v>
       </c>
       <c r="C32" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>9.1165413533834588E-2</v>
       </c>
       <c r="D32" s="95">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>0.35661334373780723</v>
       </c>
       <c r="E32" s="95">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>0.72388059701492535</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G32" s="25"/>
+      <c r="H32" s="81">
+        <v>500</v>
+      </c>
+      <c r="I32" s="107">
+        <f t="shared" si="21"/>
+        <v>1.1003102378490175</v>
+      </c>
+      <c r="J32" s="107">
+        <f t="shared" si="22"/>
+        <v>1.5542753183747724</v>
+      </c>
+      <c r="K32" s="107">
+        <f t="shared" si="23"/>
+        <v>3.6216216216216215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="104" t="s">
         <v>79</v>
       </c>
@@ -4916,48 +5137,98 @@
         <v>0.16686212557582963</v>
       </c>
       <c r="D33" s="105">
-        <f t="shared" ref="D33:E33" si="12">AVERAGE(D21,D24,D27,D30)</f>
+        <f t="shared" ref="D33:E33" si="24">AVERAGE(D21,D24,D27,D30)</f>
         <v>0.23671270916001977</v>
       </c>
       <c r="E33" s="105">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>-7.4494949494949503E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G33" s="104" t="s">
+        <v>79</v>
+      </c>
+      <c r="H33" s="101">
+        <v>1000</v>
+      </c>
+      <c r="I33" s="108">
+        <f>AVERAGE(I21,I24,I27,I30)</f>
+        <v>1.2252552577674347</v>
+      </c>
+      <c r="J33" s="108">
+        <f t="shared" ref="J33:K33" si="25">AVERAGE(J21,J24,J27,J30)</f>
+        <v>1.6399481532220546</v>
+      </c>
+      <c r="K33" s="108">
+        <f t="shared" si="25"/>
+        <v>1.1198435277382646</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="104"/>
       <c r="B34" s="102">
         <v>100</v>
       </c>
       <c r="C34" s="105">
-        <f t="shared" ref="C34:E35" si="13">AVERAGE(C22,C25,C28,C31)</f>
+        <f t="shared" ref="C34:E35" si="26">AVERAGE(C22,C25,C28,C31)</f>
         <v>0.41292162836118818</v>
       </c>
       <c r="D34" s="105">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>0.39057236964142694</v>
       </c>
       <c r="E34" s="105">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>0.61656911476296739</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G34" s="104"/>
+      <c r="H34" s="102">
+        <v>100</v>
+      </c>
+      <c r="I34" s="108">
+        <f t="shared" ref="I34:K35" si="27">AVERAGE(I22,I25,I28,I31)</f>
+        <v>1.8279848190889318</v>
+      </c>
+      <c r="J34" s="108">
+        <f t="shared" si="27"/>
+        <v>2.0223284841220992</v>
+      </c>
+      <c r="K34" s="108">
+        <f t="shared" si="27"/>
+        <v>3.4348396979975928</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="104"/>
       <c r="B35" s="103">
         <v>500</v>
       </c>
       <c r="C35" s="105">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>-0.10737297690606165</v>
       </c>
       <c r="D35" s="105">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>8.4282135931903965E-2</v>
       </c>
       <c r="E35" s="105">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>4.5793867202449268E-2</v>
+      </c>
+      <c r="G35" s="104"/>
+      <c r="H35" s="103">
+        <v>500</v>
+      </c>
+      <c r="I35" s="108">
+        <f t="shared" si="27"/>
+        <v>0.94300505018449243</v>
+      </c>
+      <c r="J35" s="108">
+        <f t="shared" si="27"/>
+        <v>1.1419166305049759</v>
+      </c>
+      <c r="K35" s="108">
+        <f t="shared" si="27"/>
+        <v>1.581518765729292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
review 2nd round - 1st and 2nd question update
</commit_message>
<xml_diff>
--- a/data/tuning_and_performance.xlsx
+++ b/data/tuning_and_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LENKA\STU\PHD\Science\self tunable HE\repository\self_tunable_HE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5730DC-CE27-4DBF-8CDC-220B61A59F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38FA4BB-0E84-46CA-83F9-DB74F3630B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-4560" windowWidth="30936" windowHeight="16776" xr2:uid="{FDE36F7A-3726-4B54-89C5-B98D2615A837}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{FDE36F7A-3726-4B54-89C5-B98D2615A837}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="85">
   <si>
     <r>
       <t>Q</t>
@@ -1104,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24187AA2-D870-438E-B038-0C0C3317218D}">
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -4394,17 +4394,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C35220-4847-41A4-99D4-689044B6F5A0}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="9.7265625" customWidth="1"/>
     <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>19</v>
       </c>
@@ -4421,7 +4422,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -4438,7 +4439,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="2">
         <v>100</v>
@@ -4453,7 +4454,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="77"/>
       <c r="B4" s="78">
         <v>500</v>
@@ -4467,8 +4468,20 @@
       <c r="E4" s="84">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15"/>
       <c r="B5" s="33" t="s">
         <v>15</v>
@@ -4482,8 +4495,23 @@
       <c r="E5" s="17">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H5" s="9">
+        <v>1000</v>
+      </c>
+      <c r="I5">
+        <f>AVERAGE(C2,C6,C10,C14)</f>
+        <v>587</v>
+      </c>
+      <c r="J5">
+        <f>AVERAGE(D2,D6,D10,D14)</f>
+        <v>0.29512499999999997</v>
+      </c>
+      <c r="K5">
+        <f>AVERAGE(E2,E6,E10,E14)</f>
+        <v>12.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="20">
         <v>2</v>
       </c>
@@ -4499,8 +4527,23 @@
       <c r="E6" s="10">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H6" s="2">
+        <v>100</v>
+      </c>
+      <c r="I6">
+        <f>AVERAGE(C3,C7,C11,C15)</f>
+        <v>818.25</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J7" si="0">AVERAGE(D3,D7,D11,D15)</f>
+        <v>0.40352500000000002</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:K8" si="1">AVERAGE(E3,E7,E11,E15)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="23"/>
       <c r="B7" s="3">
         <v>100</v>
@@ -4514,8 +4557,23 @@
       <c r="E7" s="3">
         <v>26.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H7" s="78">
+        <v>500</v>
+      </c>
+      <c r="I7">
+        <f>AVERAGE(C4,C8,C12,C16)</f>
+        <v>506.5</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0.2092</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>22.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="80"/>
       <c r="B8" s="81">
         <v>500</v>
@@ -4529,8 +4587,23 @@
       <c r="E8" s="84">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H8" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8">
+        <f>AVERAGE(C5,C9,C13,C17)</f>
+        <v>519.75</v>
+      </c>
+      <c r="J8">
+        <f>AVERAGE(D5,D9,D13,D17)</f>
+        <v>0.1885</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="25"/>
       <c r="B9" s="34" t="s">
         <v>15</v>
@@ -4545,7 +4618,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>3</v>
       </c>
@@ -4561,8 +4634,11 @@
       <c r="E10" s="9">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="I10" s="100"/>
+      <c r="J10" s="100"/>
+      <c r="K10" s="100"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
       <c r="B11" s="2">
         <v>100</v>
@@ -4577,7 +4653,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="77"/>
       <c r="B12" s="78">
         <v>500</v>
@@ -4592,7 +4668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="15"/>
       <c r="B13" s="33" t="s">
         <v>15</v>
@@ -4606,8 +4682,11 @@
       <c r="E13" s="17">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="I13" s="100"/>
+      <c r="J13" s="100"/>
+      <c r="K13" s="100"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="20">
         <v>4</v>
       </c>
@@ -4623,8 +4702,23 @@
       <c r="E14" s="21">
         <v>22.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H14" s="9">
+        <v>1000</v>
+      </c>
+      <c r="I14" s="100">
+        <f>(I5-$I$8)/$I$8</f>
+        <v>0.12938912938912939</v>
+      </c>
+      <c r="J14" s="100">
+        <f>(J5-$J$8)/$J$8</f>
+        <v>0.56564986737400513</v>
+      </c>
+      <c r="K14" s="100">
+        <f>(K5-$K$8)/$K$8</f>
+        <v>0.14772727272727273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="23"/>
       <c r="B15" s="3">
         <v>100</v>
@@ -4638,8 +4732,23 @@
       <c r="E15" s="3">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H15" s="2">
+        <v>100</v>
+      </c>
+      <c r="I15" s="100">
+        <f t="shared" ref="I15:I16" si="2">(I6-$I$8)/$I$8</f>
+        <v>0.57431457431457433</v>
+      </c>
+      <c r="J15" s="100">
+        <f t="shared" ref="J15:J16" si="3">(J6-$J$8)/$J$8</f>
+        <v>1.1407161803713528</v>
+      </c>
+      <c r="K15" s="100">
+        <f t="shared" ref="K15:K16" si="4">(K6-$K$8)/$K$8</f>
+        <v>2.6363636363636362</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="80"/>
       <c r="B16" s="81">
         <v>500</v>
@@ -4652,6 +4761,21 @@
       </c>
       <c r="E16" s="81">
         <v>67</v>
+      </c>
+      <c r="H16" s="78">
+        <v>500</v>
+      </c>
+      <c r="I16" s="100">
+        <f t="shared" si="2"/>
+        <v>-2.5493025493025494E-2</v>
+      </c>
+      <c r="J16" s="100">
+        <f t="shared" si="3"/>
+        <v>0.10981432360742703</v>
+      </c>
+      <c r="K16" s="100">
+        <f t="shared" si="4"/>
+        <v>1.0227272727272727</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4745,15 +4869,15 @@
         <v>100</v>
       </c>
       <c r="C22" s="93">
-        <f t="shared" ref="C22" si="0">(C3-$C$5)/C3</f>
+        <f t="shared" ref="C22" si="5">(C3-$C$5)/C3</f>
         <v>0.2179930795847751</v>
       </c>
       <c r="D22" s="93">
-        <f t="shared" ref="D22:D23" si="1">(D3-$D$5)/D3</f>
+        <f t="shared" ref="D22:D23" si="6">(D3-$D$5)/D3</f>
         <v>8.7687687687687699E-2</v>
       </c>
       <c r="E22" s="93">
-        <f t="shared" ref="E22:E23" si="2">(E3-$E$5)/E3</f>
+        <f t="shared" ref="E22:E23" si="7">(E3-$E$5)/E3</f>
         <v>0.24</v>
       </c>
       <c r="G22" s="13"/>
@@ -4761,15 +4885,15 @@
         <v>100</v>
       </c>
       <c r="I22" s="106">
-        <f t="shared" ref="I22" si="3">C3/$C$5</f>
+        <f t="shared" ref="I22" si="8">C3/$C$5</f>
         <v>1.2787610619469028</v>
       </c>
       <c r="J22" s="106">
-        <f t="shared" ref="J22:J23" si="4">D3/$D$5</f>
+        <f t="shared" ref="J22:J23" si="9">D3/$D$5</f>
         <v>1.0961158657011192</v>
       </c>
       <c r="K22" s="106">
-        <f t="shared" ref="K22:K23" si="5">E3/$E$5</f>
+        <f t="shared" ref="K22:K23" si="10">E3/$E$5</f>
         <v>1.3157894736842106</v>
       </c>
     </row>
@@ -4783,11 +4907,11 @@
         <v>-0.16295025728987994</v>
       </c>
       <c r="D23" s="93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.13447293447293437</v>
       </c>
       <c r="E23" s="93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>-0.26666666666666666</v>
       </c>
       <c r="G23" s="15"/>
@@ -4799,11 +4923,11 @@
         <v>0.85988200589970498</v>
       </c>
       <c r="J23" s="106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.1553653719552335</v>
       </c>
       <c r="K23" s="106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.78947368421052633</v>
       </c>
     </row>
@@ -4851,15 +4975,15 @@
         <v>100</v>
       </c>
       <c r="C25" s="95">
-        <f t="shared" ref="C25:C26" si="6">(C7-$C$9)/C7</f>
+        <f t="shared" ref="C25:C26" si="11">(C7-$C$9)/C7</f>
         <v>0.5907590759075908</v>
       </c>
       <c r="D25" s="95">
-        <f t="shared" ref="D25:D26" si="7">(D7-$D$9)/D7</f>
+        <f t="shared" ref="D25:D26" si="12">(D7-$D$9)/D7</f>
         <v>0.17720430107526888</v>
       </c>
       <c r="E25" s="95">
-        <f t="shared" ref="E25:E26" si="8">(E7-$E$9)/E7</f>
+        <f t="shared" ref="E25:E26" si="13">(E7-$E$9)/E7</f>
         <v>0.64150943396226412</v>
       </c>
       <c r="G25" s="23"/>
@@ -4867,15 +4991,15 @@
         <v>100</v>
       </c>
       <c r="I25" s="107">
-        <f t="shared" ref="I25:I26" si="9">C7/$C$9</f>
+        <f t="shared" ref="I25:I26" si="14">C7/$C$9</f>
         <v>2.443548387096774</v>
       </c>
       <c r="J25" s="107">
-        <f t="shared" ref="J25:J26" si="10">D7/$D$9</f>
+        <f t="shared" ref="J25:J26" si="15">D7/$D$9</f>
         <v>1.2153685311029796</v>
       </c>
       <c r="K25" s="107">
-        <f t="shared" ref="K25:K26" si="11">E7/$E$9</f>
+        <f t="shared" ref="K25:K26" si="16">E7/$E$9</f>
         <v>2.7894736842105261</v>
       </c>
     </row>
@@ -4885,15 +5009,15 @@
         <v>500</v>
       </c>
       <c r="C26" s="95">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-0.47619047619047616</v>
       </c>
       <c r="D26" s="95">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>-5.2255225522552302E-2</v>
       </c>
       <c r="E26" s="95">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>-0.46153846153846156</v>
       </c>
       <c r="G26" s="25"/>
@@ -4901,15 +5025,15 @@
         <v>500</v>
       </c>
       <c r="I26" s="107">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.67741935483870963</v>
       </c>
       <c r="J26" s="107">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.95033978044955558</v>
       </c>
       <c r="K26" s="107">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0.68421052631578949</v>
       </c>
     </row>
@@ -4957,15 +5081,15 @@
         <v>100</v>
       </c>
       <c r="C28" s="93">
-        <f t="shared" ref="C28:C29" si="12">(C11-$C$13)/C11</f>
+        <f t="shared" ref="C28:C29" si="17">(C11-$C$13)/C11</f>
         <v>0.53266331658291455</v>
       </c>
       <c r="D28" s="93">
-        <f t="shared" ref="D28:D29" si="13">(D11-$D$13)/D11</f>
+        <f t="shared" ref="D28:D29" si="18">(D11-$D$13)/D11</f>
         <v>0.69123556002009034</v>
       </c>
       <c r="E28" s="93">
-        <f t="shared" ref="E28:E29" si="14">(E11-$E$13)/E11</f>
+        <f t="shared" ref="E28:E29" si="19">(E11-$E$13)/E11</f>
         <v>0.79032258064516125</v>
       </c>
       <c r="G28" s="13"/>
@@ -4973,15 +5097,15 @@
         <v>100</v>
       </c>
       <c r="I28" s="106">
-        <f t="shared" ref="I28:I29" si="15">C11/$C$13</f>
+        <f t="shared" ref="I28:I29" si="20">C11/$C$13</f>
         <v>2.139784946236559</v>
       </c>
       <c r="J28" s="106">
-        <f t="shared" ref="J28:J29" si="16">D11/$D$13</f>
+        <f t="shared" ref="J28:J29" si="21">D11/$D$13</f>
         <v>3.2387149247661648</v>
       </c>
       <c r="K28" s="106">
-        <f t="shared" ref="K28:K29" si="17">E11/$E$13</f>
+        <f t="shared" ref="K28:K29" si="22">E11/$E$13</f>
         <v>4.7692307692307692</v>
       </c>
     </row>
@@ -4991,15 +5115,15 @@
         <v>500</v>
       </c>
       <c r="C29" s="93">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0.11848341232227488</v>
       </c>
       <c r="D29" s="93">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>-0.10170250896057347</v>
       </c>
       <c r="E29" s="93">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>0.1875</v>
       </c>
       <c r="G29" s="15"/>
@@ -5007,15 +5131,15 @@
         <v>500</v>
       </c>
       <c r="I29" s="106">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1.1344086021505377</v>
       </c>
       <c r="J29" s="106">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.90768605124034163</v>
       </c>
       <c r="K29" s="106">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>1.2307692307692308</v>
       </c>
     </row>
@@ -5063,15 +5187,15 @@
         <v>100</v>
       </c>
       <c r="C31" s="95">
-        <f t="shared" ref="C31:C32" si="18">(C15-$C$17)/C15</f>
+        <f t="shared" ref="C31:C32" si="23">(C15-$C$17)/C15</f>
         <v>0.3102710413694722</v>
       </c>
       <c r="D31" s="95">
-        <f t="shared" ref="D31:D32" si="19">(D15-$D$17)/D15</f>
+        <f t="shared" ref="D31:D32" si="24">(D15-$D$17)/D15</f>
         <v>0.6061619297826607</v>
       </c>
       <c r="E31" s="95">
-        <f t="shared" ref="E31:E32" si="20">(E15-$E$17)/E15</f>
+        <f t="shared" ref="E31:E32" si="25">(E15-$E$17)/E15</f>
         <v>0.7944444444444444</v>
       </c>
       <c r="G31" s="23"/>
@@ -5079,15 +5203,15 @@
         <v>100</v>
       </c>
       <c r="I31" s="107">
-        <f t="shared" ref="I31:I32" si="21">C15/$C$17</f>
+        <f t="shared" ref="I31:I32" si="26">C15/$C$17</f>
         <v>1.4498448810754911</v>
       </c>
       <c r="J31" s="107">
-        <f t="shared" ref="J31:J32" si="22">D15/$D$17</f>
+        <f t="shared" ref="J31:J32" si="27">D15/$D$17</f>
         <v>2.5391146149181325</v>
       </c>
       <c r="K31" s="107">
-        <f t="shared" ref="K31:K32" si="23">E15/$E$17</f>
+        <f t="shared" ref="K31:K32" si="28">E15/$E$17</f>
         <v>4.8648648648648649</v>
       </c>
     </row>
@@ -5097,15 +5221,15 @@
         <v>500</v>
       </c>
       <c r="C32" s="95">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>9.1165413533834588E-2</v>
       </c>
       <c r="D32" s="95">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>0.35661334373780723</v>
       </c>
       <c r="E32" s="95">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.72388059701492535</v>
       </c>
       <c r="G32" s="25"/>
@@ -5113,15 +5237,15 @@
         <v>500</v>
       </c>
       <c r="I32" s="107">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>1.1003102378490175</v>
       </c>
       <c r="J32" s="107">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>1.5542753183747724</v>
       </c>
       <c r="K32" s="107">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>3.6216216216216215</v>
       </c>
     </row>
@@ -5137,11 +5261,11 @@
         <v>0.16686212557582963</v>
       </c>
       <c r="D33" s="105">
-        <f t="shared" ref="D33:E33" si="24">AVERAGE(D21,D24,D27,D30)</f>
+        <f t="shared" ref="D33" si="29">AVERAGE(D21,D24,D27,D30)</f>
         <v>0.23671270916001977</v>
       </c>
       <c r="E33" s="105">
-        <f t="shared" si="24"/>
+        <f>AVERAGE(E21,E24,E27,E30)</f>
         <v>-7.4494949494949503E-2</v>
       </c>
       <c r="G33" s="104" t="s">
@@ -5155,11 +5279,11 @@
         <v>1.2252552577674347</v>
       </c>
       <c r="J33" s="108">
-        <f t="shared" ref="J33:K33" si="25">AVERAGE(J21,J24,J27,J30)</f>
+        <f t="shared" ref="J33" si="30">AVERAGE(J21,J24,J27,J30)</f>
         <v>1.6399481532220546</v>
       </c>
       <c r="K33" s="108">
-        <f t="shared" si="25"/>
+        <f>AVERAGE(K21,K24,K27,K30)</f>
         <v>1.1198435277382646</v>
       </c>
     </row>
@@ -5169,15 +5293,15 @@
         <v>100</v>
       </c>
       <c r="C34" s="105">
-        <f t="shared" ref="C34:E35" si="26">AVERAGE(C22,C25,C28,C31)</f>
+        <f t="shared" ref="C34:E35" si="31">AVERAGE(C22,C25,C28,C31)</f>
         <v>0.41292162836118818</v>
       </c>
       <c r="D34" s="105">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.39057236964142694</v>
       </c>
       <c r="E34" s="105">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.61656911476296739</v>
       </c>
       <c r="G34" s="104"/>
@@ -5185,15 +5309,15 @@
         <v>100</v>
       </c>
       <c r="I34" s="108">
-        <f t="shared" ref="I34:K35" si="27">AVERAGE(I22,I25,I28,I31)</f>
+        <f t="shared" ref="I34:K35" si="32">AVERAGE(I22,I25,I28,I31)</f>
         <v>1.8279848190889318</v>
       </c>
       <c r="J34" s="108">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>2.0223284841220992</v>
       </c>
       <c r="K34" s="108">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>3.4348396979975928</v>
       </c>
     </row>
@@ -5203,15 +5327,15 @@
         <v>500</v>
       </c>
       <c r="C35" s="105">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>-0.10737297690606165</v>
       </c>
       <c r="D35" s="105">
-        <f t="shared" si="26"/>
+        <f>AVERAGE(D23,D26,D29,D32)</f>
         <v>8.4282135931903965E-2</v>
       </c>
       <c r="E35" s="105">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>4.5793867202449268E-2</v>
       </c>
       <c r="G35" s="104"/>
@@ -5219,15 +5343,15 @@
         <v>500</v>
       </c>
       <c r="I35" s="108">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0.94300505018449243</v>
       </c>
       <c r="J35" s="108">
-        <f t="shared" si="27"/>
+        <f>AVERAGE(J23,J26,J29,J32)</f>
         <v>1.1419166305049759</v>
       </c>
       <c r="K35" s="108">
-        <f t="shared" si="27"/>
+        <f>AVERAGE(K23,K26,K29,K32)</f>
         <v>1.581518765729292</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new way of relative improvement evaluation
</commit_message>
<xml_diff>
--- a/data/tuning_and_performance.xlsx
+++ b/data/tuning_and_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LENKA\STU\PHD\Science\self tunable HE\repository\self_tunable_HE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38FA4BB-0E84-46CA-83F9-DB74F3630B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31ABC44-127E-4F7D-BD95-9A8F3050F574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{FDE36F7A-3726-4B54-89C5-B98D2615A837}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FDE36F7A-3726-4B54-89C5-B98D2615A837}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -666,7 +666,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -764,7 +764,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
@@ -786,6 +785,8 @@
     <xf numFmtId="43" fontId="0" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Čiarka" xfId="2" builtinId="3"/>
@@ -1104,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24187AA2-D870-438E-B038-0C0C3317218D}">
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1667,15 +1668,15 @@
       <c r="B35" s="9">
         <v>1000</v>
       </c>
-      <c r="C35" s="93">
+      <c r="C35" s="92">
         <f>(C16-$C$19)/$C$19</f>
         <v>5.3097345132743362E-2</v>
       </c>
-      <c r="D35" s="93">
+      <c r="D35" s="92">
         <f>(D16-$D$19)/$D$19</f>
         <v>1.2053982883475971</v>
       </c>
-      <c r="E35" s="93">
+      <c r="E35" s="92">
         <f>(F16-$F$19)/$F$19</f>
         <v>0.73684210526315785</v>
       </c>
@@ -1685,33 +1686,33 @@
       <c r="B36" s="2">
         <v>100</v>
       </c>
-      <c r="C36" s="93">
+      <c r="C36" s="92">
         <f>(C17-$C$19)/$C$19</f>
         <v>0.27876106194690264</v>
       </c>
-      <c r="D36" s="93">
+      <c r="D36" s="92">
         <f>(D17-$D$19)/$D$19</f>
         <v>9.6115865701119171E-2</v>
       </c>
-      <c r="E36" s="93">
+      <c r="E36" s="92">
         <f>(F17-$F$19)/$F$19</f>
         <v>0.31578947368421051</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="88"/>
-      <c r="B37" s="89">
+      <c r="A37" s="87"/>
+      <c r="B37" s="88">
         <v>500</v>
       </c>
-      <c r="C37" s="93">
+      <c r="C37" s="92">
         <f>(C18-$C$19)/$C$19</f>
         <v>-0.14011799410029499</v>
       </c>
-      <c r="D37" s="94">
+      <c r="D37" s="93">
         <f>(D18-$D$19)/$D$19</f>
         <v>0.15536537195523359</v>
       </c>
-      <c r="E37" s="93">
+      <c r="E37" s="92">
         <f>(F18-$F$19)/$F$19</f>
         <v>-0.21052631578947367</v>
       </c>
@@ -1723,15 +1724,15 @@
       <c r="B38" s="21">
         <v>1000</v>
       </c>
-      <c r="C38" s="95">
+      <c r="C38" s="94">
         <f>(C20-$C$23)/$C$23</f>
         <v>0.47177419354838712</v>
       </c>
-      <c r="D38" s="95">
+      <c r="D38" s="94">
         <f>(D20-$D$23)/$D$23</f>
         <v>1.467328802927339</v>
       </c>
-      <c r="E38" s="95">
+      <c r="E38" s="94">
         <f>(F20-$F$23)/$F$23</f>
         <v>-0.47368421052631576</v>
       </c>
@@ -1741,33 +1742,33 @@
       <c r="B39" s="3">
         <v>100</v>
       </c>
-      <c r="C39" s="95">
+      <c r="C39" s="94">
         <f>(C21-$C$23)/$C$23</f>
         <v>1.4435483870967742</v>
       </c>
-      <c r="D39" s="95">
+      <c r="D39" s="94">
         <f>(D21-$D$23)/$D$23</f>
         <v>0.21536853110297968</v>
       </c>
-      <c r="E39" s="95">
+      <c r="E39" s="94">
         <f>(F21-$F$23)/$F$23</f>
         <v>1.7894736842105263</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="90"/>
-      <c r="B40" s="91">
+      <c r="A40" s="89"/>
+      <c r="B40" s="90">
         <v>500</v>
       </c>
-      <c r="C40" s="95">
+      <c r="C40" s="94">
         <f>(C22-$C$23)/$C$23</f>
         <v>-0.32258064516129031</v>
       </c>
-      <c r="D40" s="95">
+      <c r="D40" s="94">
         <f>(D22-$D$23)/$D$23</f>
         <v>-4.9660219550444376E-2</v>
       </c>
-      <c r="E40" s="95">
+      <c r="E40" s="94">
         <f>(F22-$F$23)/$F$23</f>
         <v>-0.31578947368421051</v>
       </c>
@@ -1779,15 +1780,15 @@
       <c r="B41" s="9">
         <v>1000</v>
       </c>
-      <c r="C41" s="93">
+      <c r="C41" s="92">
         <f>(C24-$C$27)/$C$27</f>
         <v>0.31720430107526881</v>
       </c>
-      <c r="D41" s="93">
+      <c r="D41" s="92">
         <f>(D24-$D$27)/$D$27</f>
         <v>-0.23058153721024807</v>
       </c>
-      <c r="E41" s="93">
+      <c r="E41" s="92">
         <f>(F24-$F$27)/$F$27</f>
         <v>0</v>
       </c>
@@ -1797,33 +1798,33 @@
       <c r="B42" s="2">
         <v>100</v>
       </c>
-      <c r="C42" s="93">
+      <c r="C42" s="92">
         <f>(C25-$C$27)/$C$27</f>
         <v>1.1397849462365592</v>
       </c>
-      <c r="D42" s="93">
+      <c r="D42" s="92">
         <f>(D25-$D$27)/$D$27</f>
         <v>2.2387149247661648</v>
       </c>
-      <c r="E42" s="93">
+      <c r="E42" s="92">
         <f>(F25-$F$27)/$F$27</f>
         <v>3.7692307692307692</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="88"/>
-      <c r="B43" s="89">
+      <c r="A43" s="87"/>
+      <c r="B43" s="88">
         <v>500</v>
       </c>
-      <c r="C43" s="94">
+      <c r="C43" s="93">
         <f>(C26-$C$27)/$C$27</f>
         <v>0.13440860215053763</v>
       </c>
-      <c r="D43" s="93">
+      <c r="D43" s="92">
         <f>(D26-$D$27)/$D$27</f>
         <v>-9.2313948759658385E-2</v>
       </c>
-      <c r="E43" s="94">
+      <c r="E43" s="93">
         <f>(F26-$F$27)/$F$27</f>
         <v>0.23076923076923078</v>
       </c>
@@ -1835,15 +1836,15 @@
       <c r="B44" s="21">
         <v>1000</v>
       </c>
-      <c r="C44" s="95">
+      <c r="C44" s="94">
         <f>(C28-$C$31)/$C$31</f>
         <v>5.894519131334023E-2</v>
       </c>
-      <c r="D44" s="95">
+      <c r="D44" s="94">
         <f>(D28-$D$31)/$D$31</f>
         <v>0.11764705882352942</v>
       </c>
-      <c r="E44" s="95">
+      <c r="E44" s="94">
         <f>(F28-$F$31)/$F$31</f>
         <v>0.21621621621621623</v>
       </c>
@@ -1853,33 +1854,33 @@
       <c r="B45" s="3">
         <v>100</v>
       </c>
-      <c r="C45" s="95">
+      <c r="C45" s="94">
         <f>(C29-$C$31)/$C$31</f>
         <v>0.4498448810754912</v>
       </c>
-      <c r="D45" s="95">
+      <c r="D45" s="94">
         <f>(D29-$D$31)/$D$31</f>
         <v>1.5391146149181325</v>
       </c>
-      <c r="E45" s="95">
+      <c r="E45" s="94">
         <f>(F29-$F$31)/$F$31</f>
         <v>3.8648648648648649</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="92"/>
+      <c r="A46" s="91"/>
       <c r="B46" s="1">
         <v>500</v>
       </c>
-      <c r="C46" s="96">
+      <c r="C46" s="95">
         <f>(C30-$C$31)/$C$31</f>
         <v>0.10031023784901758</v>
       </c>
-      <c r="D46" s="96">
+      <c r="D46" s="95">
         <f>(D30-$D$31)/$D$31</f>
         <v>0.55427531837477251</v>
       </c>
-      <c r="E46" s="96">
+      <c r="E46" s="95">
         <f>(F30-$F$31)/$F$31</f>
         <v>2.6216216216216215</v>
       </c>
@@ -2080,15 +2081,15 @@
       <c r="B60" s="9">
         <v>1000</v>
       </c>
-      <c r="C60" s="62">
-        <f t="shared" ref="C60:E61" si="4">AVERAGE(C49,C51,C53,C55)</f>
+      <c r="C60" s="106">
+        <f>AVERAGE(C49,C51,C53,C55)</f>
         <v>22.525525776743486</v>
       </c>
-      <c r="D60" s="62">
-        <f t="shared" si="4"/>
+      <c r="D60" s="106">
+        <f t="shared" ref="C60:E61" si="4">AVERAGE(D49,D51,D53,D55)</f>
         <v>63.99481532220544</v>
       </c>
-      <c r="E60" s="62">
+      <c r="E60" s="106">
         <f t="shared" si="4"/>
         <v>11.984352773826457</v>
       </c>
@@ -2098,15 +2099,15 @@
       <c r="B61" s="86">
         <v>100</v>
       </c>
-      <c r="C61" s="87">
+      <c r="C61" s="109">
         <f t="shared" si="4"/>
         <v>82.79848190889318</v>
       </c>
-      <c r="D61" s="87">
+      <c r="D61" s="109">
         <f t="shared" si="4"/>
         <v>102.2328484122099</v>
       </c>
-      <c r="E61" s="87">
+      <c r="E61" s="109">
         <f t="shared" si="4"/>
         <v>243.48396979975928</v>
       </c>
@@ -2116,15 +2117,15 @@
       <c r="B62" s="37">
         <v>500</v>
       </c>
-      <c r="C62" s="87">
+      <c r="C62" s="108">
         <f>AVERAGE(C37,C40,C43,C46)</f>
         <v>-5.6994949815507519E-2</v>
       </c>
-      <c r="D62" s="87">
+      <c r="D62" s="108">
         <f>AVERAGE(D37,D40,D43,D46)</f>
         <v>0.14191663050497583</v>
       </c>
-      <c r="E62" s="87">
+      <c r="E62" s="108">
         <f>AVERAGE(E37,E40,E43,E46)</f>
         <v>0.58151876572929206</v>
       </c>
@@ -2957,7 +2958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCC6C2E-BC1D-47B4-A935-B6D151C5A89E}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
@@ -3309,7 +3310,7 @@
         <f>(MIN(E16:E17)-E18)/MIN(E16:E17)</f>
         <v>8.7687687687687699E-2</v>
       </c>
-      <c r="N18" s="97">
+      <c r="N18" s="96">
         <f>(MIN(G16:G17)-G18)/MIN(G16:G17)</f>
         <v>-0.12264150943396215</v>
       </c>
@@ -3421,7 +3422,7 @@
         <f>(MIN(E19:E20)-E21)/MIN(E19:E20)</f>
         <v>0.17720430107526888</v>
       </c>
-      <c r="N21" s="97">
+      <c r="N21" s="96">
         <f t="shared" ref="N21:N27" si="0">(MIN(G19:G20)-G21)/MIN(G19:G20)</f>
         <v>-0.34538152610441758</v>
       </c>
@@ -3533,7 +3534,7 @@
         <f>(MIN(E22:E23)-E24)/MIN(E22:E23)</f>
         <v>-0.29968287526427062</v>
       </c>
-      <c r="N24" s="97">
+      <c r="N24" s="96">
         <f t="shared" si="0"/>
         <v>-4.4776119402985232E-2</v>
       </c>
@@ -3723,15 +3724,15 @@
       <c r="K31" s="8">
         <v>1</v>
       </c>
-      <c r="L31" s="93">
+      <c r="L31" s="92">
         <f>(C16-$C$18)/C16</f>
         <v>5.0420168067226892E-2</v>
       </c>
-      <c r="M31" s="93">
+      <c r="M31" s="92">
         <f>(E16-$E$18)/E16</f>
         <v>0.54656716417910445</v>
       </c>
-      <c r="N31" s="93">
+      <c r="N31" s="92">
         <f>(I16-$I$18)/I16</f>
         <v>0.42424242424242425</v>
       </c>
@@ -3757,15 +3758,15 @@
       </c>
       <c r="G32" s="43"/>
       <c r="K32" s="13"/>
-      <c r="L32" s="93">
+      <c r="L32" s="92">
         <f>(C17-$C$18)/C17</f>
         <v>0.2179930795847751</v>
       </c>
-      <c r="M32" s="93">
+      <c r="M32" s="92">
         <f>(E17-$E$18)/E17</f>
         <v>8.7687687687687699E-2</v>
       </c>
-      <c r="N32" s="93">
+      <c r="N32" s="92">
         <f>(I17-$I$18)/I17</f>
         <v>0.24</v>
       </c>
@@ -3789,9 +3790,9 @@
       </c>
       <c r="G33" s="47"/>
       <c r="K33" s="15"/>
-      <c r="L33" s="93"/>
-      <c r="M33" s="93"/>
-      <c r="N33" s="93"/>
+      <c r="L33" s="92"/>
+      <c r="M33" s="92"/>
+      <c r="N33" s="92"/>
     </row>
     <row r="34" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="48"/>
@@ -3814,15 +3815,15 @@
       <c r="K34" s="20">
         <v>2</v>
       </c>
-      <c r="L34" s="95">
+      <c r="L34" s="94">
         <f>(C19-$C$21)/C19</f>
         <v>0.32054794520547947</v>
       </c>
-      <c r="M34" s="95">
+      <c r="M34" s="94">
         <f>(E19-$E$21)/E19</f>
         <v>0.59470338983050841</v>
       </c>
-      <c r="N34" s="95">
+      <c r="N34" s="94">
         <f>(I19-$I$21)/I19</f>
         <v>-0.9</v>
       </c>
@@ -3848,15 +3849,15 @@
       </c>
       <c r="G35" s="53"/>
       <c r="K35" s="23"/>
-      <c r="L35" s="95">
+      <c r="L35" s="94">
         <f>(C20-$C$21)/C20</f>
         <v>0.5907590759075908</v>
       </c>
-      <c r="M35" s="95">
+      <c r="M35" s="94">
         <f>(E20-$E$21)/E20</f>
         <v>0.17720430107526888</v>
       </c>
-      <c r="N35" s="95">
+      <c r="N35" s="94">
         <f>(I20-$I$21)/I20</f>
         <v>0.64150943396226412</v>
       </c>
@@ -3880,9 +3881,9 @@
       </c>
       <c r="G36" s="47"/>
       <c r="K36" s="25"/>
-      <c r="L36" s="95"/>
-      <c r="M36" s="99"/>
-      <c r="N36" s="95"/>
+      <c r="L36" s="94"/>
+      <c r="M36" s="98"/>
+      <c r="N36" s="94"/>
     </row>
     <row r="37" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="48"/>
@@ -3905,15 +3906,15 @@
       <c r="K37" s="8">
         <v>3</v>
       </c>
-      <c r="L37" s="93">
+      <c r="L37" s="92">
         <f>(C22-$C$24)/C22</f>
         <v>0.24081632653061225</v>
       </c>
-      <c r="M37" s="93">
+      <c r="M37" s="92">
         <f>(E22-$E$24)/E22</f>
         <v>-0.29968287526427062</v>
       </c>
-      <c r="N37" s="93">
+      <c r="N37" s="92">
         <f>(I22-$I$24)/I22</f>
         <v>0</v>
       </c>
@@ -3939,15 +3940,15 @@
       </c>
       <c r="G38" s="43"/>
       <c r="K38" s="13"/>
-      <c r="L38" s="93">
+      <c r="L38" s="92">
         <f>(C23-$C$24)/C23</f>
         <v>0.53266331658291455</v>
       </c>
-      <c r="M38" s="93">
+      <c r="M38" s="92">
         <f>(E23-$E$24)/E23</f>
         <v>0.69123556002009034</v>
       </c>
-      <c r="N38" s="93">
+      <c r="N38" s="92">
         <f>(I23-$I$24)/I23</f>
         <v>0.79032258064516125</v>
       </c>
@@ -3971,9 +3972,9 @@
       </c>
       <c r="G39" s="47"/>
       <c r="K39" s="15"/>
-      <c r="L39" s="93"/>
-      <c r="M39" s="93"/>
-      <c r="N39" s="93"/>
+      <c r="L39" s="92"/>
+      <c r="M39" s="92"/>
+      <c r="N39" s="92"/>
     </row>
     <row r="40" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="48"/>
@@ -3996,15 +3997,15 @@
       <c r="K40" s="20">
         <v>4</v>
       </c>
-      <c r="L40" s="95">
+      <c r="L40" s="94">
         <f>(C25-$C$27)/C25</f>
         <v>5.56640625E-2</v>
       </c>
-      <c r="M40" s="95">
+      <c r="M40" s="94">
         <f>(E25-$E$27)/E25</f>
         <v>0.10526315789473685</v>
       </c>
-      <c r="N40" s="95">
+      <c r="N40" s="94">
         <f>(I25-$I$27)/I25</f>
         <v>0.17777777777777778</v>
       </c>
@@ -4030,15 +4031,15 @@
       </c>
       <c r="G41" s="53"/>
       <c r="K41" s="23"/>
-      <c r="L41" s="95">
+      <c r="L41" s="94">
         <f>(C26-$C$27)/C26</f>
         <v>0.3102710413694722</v>
       </c>
-      <c r="M41" s="95">
+      <c r="M41" s="94">
         <f>(E26-$E$27)/E26</f>
         <v>0.6061619297826607</v>
       </c>
-      <c r="N41" s="95">
+      <c r="N41" s="94">
         <f>(I26-$I$27)/I26</f>
         <v>0.7944444444444444</v>
       </c>
@@ -4062,9 +4063,9 @@
       </c>
       <c r="G42" s="47"/>
       <c r="K42" s="25"/>
-      <c r="L42" s="98"/>
-      <c r="M42" s="98"/>
-      <c r="N42" s="98"/>
+      <c r="L42" s="97"/>
+      <c r="M42" s="97"/>
+      <c r="N42" s="97"/>
     </row>
     <row r="43" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="48"/>
@@ -4087,30 +4088,30 @@
       <c r="K43" t="s">
         <v>79</v>
       </c>
-      <c r="L43" s="100">
+      <c r="L43" s="99">
         <f t="shared" ref="L43:N44" si="3">AVERAGE(L31,L34,L37,L40)</f>
         <v>0.16686212557582963</v>
       </c>
-      <c r="M43" s="100">
+      <c r="M43" s="99">
         <f t="shared" si="3"/>
         <v>0.23671270916001977</v>
       </c>
-      <c r="N43" s="100">
+      <c r="N43" s="99">
         <f t="shared" si="3"/>
         <v>-7.4494949494949503E-2</v>
       </c>
       <c r="O43" s="76"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="L44" s="100">
+      <c r="L44" s="99">
         <f t="shared" si="3"/>
         <v>0.41292162836118818</v>
       </c>
-      <c r="M44" s="100">
+      <c r="M44" s="99">
         <f t="shared" si="3"/>
         <v>0.39057236964142694</v>
       </c>
-      <c r="N44" s="100">
+      <c r="N44" s="99">
         <f t="shared" si="3"/>
         <v>0.61656911476296739</v>
       </c>
@@ -4394,8 +4395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C35220-4847-41A4-99D4-689044B6F5A0}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4634,9 +4635,9 @@
       <c r="E10" s="9">
         <v>6.5</v>
       </c>
-      <c r="I10" s="100"/>
-      <c r="J10" s="100"/>
-      <c r="K10" s="100"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="99"/>
+      <c r="K10" s="99"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
@@ -4682,9 +4683,9 @@
       <c r="E13" s="17">
         <v>6.5</v>
       </c>
-      <c r="I13" s="100"/>
-      <c r="J13" s="100"/>
-      <c r="K13" s="100"/>
+      <c r="I13" s="99"/>
+      <c r="J13" s="99"/>
+      <c r="K13" s="99"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="20">
@@ -4705,15 +4706,15 @@
       <c r="H14" s="9">
         <v>1000</v>
       </c>
-      <c r="I14" s="100">
+      <c r="I14" s="99">
         <f>(I5-$I$8)/$I$8</f>
         <v>0.12938912938912939</v>
       </c>
-      <c r="J14" s="100">
+      <c r="J14" s="99">
         <f>(J5-$J$8)/$J$8</f>
         <v>0.56564986737400513</v>
       </c>
-      <c r="K14" s="100">
+      <c r="K14" s="99">
         <f>(K5-$K$8)/$K$8</f>
         <v>0.14772727272727273</v>
       </c>
@@ -4735,15 +4736,15 @@
       <c r="H15" s="2">
         <v>100</v>
       </c>
-      <c r="I15" s="100">
+      <c r="I15" s="99">
         <f t="shared" ref="I15:I16" si="2">(I6-$I$8)/$I$8</f>
         <v>0.57431457431457433</v>
       </c>
-      <c r="J15" s="100">
+      <c r="J15" s="99">
         <f t="shared" ref="J15:J16" si="3">(J6-$J$8)/$J$8</f>
         <v>1.1407161803713528</v>
       </c>
-      <c r="K15" s="100">
+      <c r="K15" s="99">
         <f t="shared" ref="K15:K16" si="4">(K6-$K$8)/$K$8</f>
         <v>2.6363636363636362</v>
       </c>
@@ -4765,15 +4766,15 @@
       <c r="H16" s="78">
         <v>500</v>
       </c>
-      <c r="I16" s="100">
+      <c r="I16" s="99">
         <f t="shared" si="2"/>
         <v>-2.5493025493025494E-2</v>
       </c>
-      <c r="J16" s="100">
+      <c r="J16" s="99">
         <f t="shared" si="3"/>
         <v>0.10981432360742703</v>
       </c>
-      <c r="K16" s="100">
+      <c r="K16" s="99">
         <f t="shared" si="4"/>
         <v>1.0227272727272727</v>
       </c>
@@ -4832,15 +4833,15 @@
       <c r="B21" s="9">
         <v>1000</v>
       </c>
-      <c r="C21" s="93">
+      <c r="C21" s="92">
         <f>(C2-$C$5)/C2</f>
         <v>5.0420168067226892E-2</v>
       </c>
-      <c r="D21" s="93">
+      <c r="D21" s="92">
         <f>(D2-$D$5)/D2</f>
         <v>0.54656716417910445</v>
       </c>
-      <c r="E21" s="93">
+      <c r="E21" s="92">
         <f>(E2-$E$5)/E2</f>
         <v>0.42424242424242425</v>
       </c>
@@ -4850,15 +4851,15 @@
       <c r="H21" s="9">
         <v>1000</v>
       </c>
-      <c r="I21" s="106">
+      <c r="I21" s="105">
         <f>C2/$C$5</f>
         <v>1.0530973451327434</v>
       </c>
-      <c r="J21" s="106">
+      <c r="J21" s="105">
         <f>D2/$D$5</f>
         <v>2.2053982883475971</v>
       </c>
-      <c r="K21" s="106">
+      <c r="K21" s="105">
         <f>E2/$E$5</f>
         <v>1.736842105263158</v>
       </c>
@@ -4868,15 +4869,15 @@
       <c r="B22" s="2">
         <v>100</v>
       </c>
-      <c r="C22" s="93">
+      <c r="C22" s="92">
         <f t="shared" ref="C22" si="5">(C3-$C$5)/C3</f>
         <v>0.2179930795847751</v>
       </c>
-      <c r="D22" s="93">
+      <c r="D22" s="92">
         <f t="shared" ref="D22:D23" si="6">(D3-$D$5)/D3</f>
         <v>8.7687687687687699E-2</v>
       </c>
-      <c r="E22" s="93">
+      <c r="E22" s="92">
         <f t="shared" ref="E22:E23" si="7">(E3-$E$5)/E3</f>
         <v>0.24</v>
       </c>
@@ -4884,16 +4885,16 @@
       <c r="H22" s="2">
         <v>100</v>
       </c>
-      <c r="I22" s="106">
-        <f t="shared" ref="I22" si="8">C3/$C$5</f>
+      <c r="I22" s="105">
+        <f>C3/$C$5</f>
         <v>1.2787610619469028</v>
       </c>
-      <c r="J22" s="106">
-        <f t="shared" ref="J22:J23" si="9">D3/$D$5</f>
+      <c r="J22" s="105">
+        <f t="shared" ref="J22:J23" si="8">D3/$D$5</f>
         <v>1.0961158657011192</v>
       </c>
-      <c r="K22" s="106">
-        <f t="shared" ref="K22:K23" si="10">E3/$E$5</f>
+      <c r="K22" s="105">
+        <f t="shared" ref="K22:K23" si="9">E3/$E$5</f>
         <v>1.3157894736842106</v>
       </c>
     </row>
@@ -4902,15 +4903,15 @@
       <c r="B23" s="78">
         <v>500</v>
       </c>
-      <c r="C23" s="93">
+      <c r="C23" s="92">
         <f>(C4-$C$5)/C4</f>
         <v>-0.16295025728987994</v>
       </c>
-      <c r="D23" s="93">
+      <c r="D23" s="92">
         <f t="shared" si="6"/>
         <v>0.13447293447293437</v>
       </c>
-      <c r="E23" s="93">
+      <c r="E23" s="92">
         <f t="shared" si="7"/>
         <v>-0.26666666666666666</v>
       </c>
@@ -4918,16 +4919,16 @@
       <c r="H23" s="78">
         <v>500</v>
       </c>
-      <c r="I23" s="106">
+      <c r="I23" s="105">
         <f>C4/$C$5</f>
         <v>0.85988200589970498</v>
       </c>
-      <c r="J23" s="106">
+      <c r="J23" s="105">
+        <f t="shared" si="8"/>
+        <v>1.1553653719552335</v>
+      </c>
+      <c r="K23" s="105">
         <f t="shared" si="9"/>
-        <v>1.1553653719552335</v>
-      </c>
-      <c r="K23" s="106">
-        <f t="shared" si="10"/>
         <v>0.78947368421052633</v>
       </c>
     </row>
@@ -4938,15 +4939,15 @@
       <c r="B24" s="21">
         <v>1000</v>
       </c>
-      <c r="C24" s="95">
+      <c r="C24" s="94">
         <f>(C6-$C$9)/C6</f>
         <v>0.32054794520547947</v>
       </c>
-      <c r="D24" s="95">
+      <c r="D24" s="94">
         <f>(D6-$D$9)/D6</f>
         <v>0.59470338983050841</v>
       </c>
-      <c r="E24" s="95">
+      <c r="E24" s="94">
         <f>(E6-$E$9)/E6</f>
         <v>-0.9</v>
       </c>
@@ -4956,15 +4957,15 @@
       <c r="H24" s="21">
         <v>1000</v>
       </c>
-      <c r="I24" s="107">
+      <c r="I24" s="106">
         <f>C6/$C$9</f>
         <v>1.471774193548387</v>
       </c>
-      <c r="J24" s="107">
+      <c r="J24" s="106">
         <f>D6/$D$9</f>
         <v>2.467328802927339</v>
       </c>
-      <c r="K24" s="107">
+      <c r="K24" s="106">
         <f>E6/$E$9</f>
         <v>0.52631578947368418</v>
       </c>
@@ -4974,32 +4975,32 @@
       <c r="B25" s="3">
         <v>100</v>
       </c>
-      <c r="C25" s="95">
-        <f t="shared" ref="C25:C26" si="11">(C7-$C$9)/C7</f>
+      <c r="C25" s="94">
+        <f t="shared" ref="C25:C26" si="10">(C7-$C$9)/C7</f>
         <v>0.5907590759075908</v>
       </c>
-      <c r="D25" s="95">
-        <f t="shared" ref="D25:D26" si="12">(D7-$D$9)/D7</f>
+      <c r="D25" s="94">
+        <f t="shared" ref="D25:D26" si="11">(D7-$D$9)/D7</f>
         <v>0.17720430107526888</v>
       </c>
-      <c r="E25" s="95">
-        <f t="shared" ref="E25:E26" si="13">(E7-$E$9)/E7</f>
+      <c r="E25" s="94">
+        <f t="shared" ref="E25:E26" si="12">(E7-$E$9)/E7</f>
         <v>0.64150943396226412</v>
       </c>
       <c r="G25" s="23"/>
       <c r="H25" s="3">
         <v>100</v>
       </c>
-      <c r="I25" s="107">
-        <f t="shared" ref="I25:I26" si="14">C7/$C$9</f>
+      <c r="I25" s="106">
+        <f t="shared" ref="I25:I26" si="13">C7/$C$9</f>
         <v>2.443548387096774</v>
       </c>
-      <c r="J25" s="107">
-        <f t="shared" ref="J25:J26" si="15">D7/$D$9</f>
+      <c r="J25" s="106">
+        <f t="shared" ref="J25:J26" si="14">D7/$D$9</f>
         <v>1.2153685311029796</v>
       </c>
-      <c r="K25" s="107">
-        <f t="shared" ref="K25:K26" si="16">E7/$E$9</f>
+      <c r="K25" s="106">
+        <f t="shared" ref="K25:K26" si="15">E7/$E$9</f>
         <v>2.7894736842105261</v>
       </c>
     </row>
@@ -5008,32 +5009,32 @@
       <c r="B26" s="81">
         <v>500</v>
       </c>
-      <c r="C26" s="95">
+      <c r="C26" s="94">
+        <f t="shared" si="10"/>
+        <v>-0.47619047619047616</v>
+      </c>
+      <c r="D26" s="94">
         <f t="shared" si="11"/>
-        <v>-0.47619047619047616</v>
-      </c>
-      <c r="D26" s="95">
+        <v>-5.2255225522552302E-2</v>
+      </c>
+      <c r="E26" s="94">
         <f t="shared" si="12"/>
-        <v>-5.2255225522552302E-2</v>
-      </c>
-      <c r="E26" s="95">
-        <f t="shared" si="13"/>
         <v>-0.46153846153846156</v>
       </c>
       <c r="G26" s="25"/>
       <c r="H26" s="81">
         <v>500</v>
       </c>
-      <c r="I26" s="107">
+      <c r="I26" s="106">
+        <f t="shared" si="13"/>
+        <v>0.67741935483870963</v>
+      </c>
+      <c r="J26" s="106">
         <f t="shared" si="14"/>
-        <v>0.67741935483870963</v>
-      </c>
-      <c r="J26" s="107">
+        <v>0.95033978044955558</v>
+      </c>
+      <c r="K26" s="106">
         <f t="shared" si="15"/>
-        <v>0.95033978044955558</v>
-      </c>
-      <c r="K26" s="107">
-        <f t="shared" si="16"/>
         <v>0.68421052631578949</v>
       </c>
     </row>
@@ -5044,15 +5045,15 @@
       <c r="B27" s="9">
         <v>1000</v>
       </c>
-      <c r="C27" s="93">
+      <c r="C27" s="92">
         <f>(C10-$C$13)/C10</f>
         <v>0.24081632653061225</v>
       </c>
-      <c r="D27" s="93">
+      <c r="D27" s="92">
         <f>(D10-$D$13)/D10</f>
         <v>-0.29968287526427062</v>
       </c>
-      <c r="E27" s="93">
+      <c r="E27" s="92">
         <f>(E10-$E$13)/E10</f>
         <v>0</v>
       </c>
@@ -5062,15 +5063,15 @@
       <c r="H27" s="9">
         <v>1000</v>
       </c>
-      <c r="I27" s="106">
+      <c r="I27" s="105">
         <f>C10/$C$13</f>
         <v>1.3172043010752688</v>
       </c>
-      <c r="J27" s="106">
+      <c r="J27" s="105">
         <f>D10/$D$13</f>
         <v>0.7694184627897519</v>
       </c>
-      <c r="K27" s="106">
+      <c r="K27" s="105">
         <f>E10/$E$13</f>
         <v>1</v>
       </c>
@@ -5080,32 +5081,32 @@
       <c r="B28" s="2">
         <v>100</v>
       </c>
-      <c r="C28" s="93">
-        <f t="shared" ref="C28:C29" si="17">(C11-$C$13)/C11</f>
+      <c r="C28" s="92">
+        <f t="shared" ref="C28:C29" si="16">(C11-$C$13)/C11</f>
         <v>0.53266331658291455</v>
       </c>
-      <c r="D28" s="93">
-        <f t="shared" ref="D28:D29" si="18">(D11-$D$13)/D11</f>
+      <c r="D28" s="92">
+        <f t="shared" ref="D28:D29" si="17">(D11-$D$13)/D11</f>
         <v>0.69123556002009034</v>
       </c>
-      <c r="E28" s="93">
-        <f t="shared" ref="E28:E29" si="19">(E11-$E$13)/E11</f>
+      <c r="E28" s="92">
+        <f t="shared" ref="E28:E29" si="18">(E11-$E$13)/E11</f>
         <v>0.79032258064516125</v>
       </c>
       <c r="G28" s="13"/>
       <c r="H28" s="2">
         <v>100</v>
       </c>
-      <c r="I28" s="106">
-        <f t="shared" ref="I28:I29" si="20">C11/$C$13</f>
+      <c r="I28" s="105">
+        <f t="shared" ref="I28:I29" si="19">C11/$C$13</f>
         <v>2.139784946236559</v>
       </c>
-      <c r="J28" s="106">
-        <f t="shared" ref="J28:J29" si="21">D11/$D$13</f>
+      <c r="J28" s="105">
+        <f t="shared" ref="J28:J29" si="20">D11/$D$13</f>
         <v>3.2387149247661648</v>
       </c>
-      <c r="K28" s="106">
-        <f t="shared" ref="K28:K29" si="22">E11/$E$13</f>
+      <c r="K28" s="105">
+        <f t="shared" ref="K28:K29" si="21">E11/$E$13</f>
         <v>4.7692307692307692</v>
       </c>
     </row>
@@ -5114,32 +5115,32 @@
       <c r="B29" s="78">
         <v>500</v>
       </c>
-      <c r="C29" s="93">
+      <c r="C29" s="92">
+        <f t="shared" si="16"/>
+        <v>0.11848341232227488</v>
+      </c>
+      <c r="D29" s="92">
         <f t="shared" si="17"/>
-        <v>0.11848341232227488</v>
-      </c>
-      <c r="D29" s="93">
+        <v>-0.10170250896057347</v>
+      </c>
+      <c r="E29" s="92">
         <f t="shared" si="18"/>
-        <v>-0.10170250896057347</v>
-      </c>
-      <c r="E29" s="93">
-        <f t="shared" si="19"/>
         <v>0.1875</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="78">
         <v>500</v>
       </c>
-      <c r="I29" s="106">
+      <c r="I29" s="105">
+        <f t="shared" si="19"/>
+        <v>1.1344086021505377</v>
+      </c>
+      <c r="J29" s="105">
         <f t="shared" si="20"/>
-        <v>1.1344086021505377</v>
-      </c>
-      <c r="J29" s="106">
+        <v>0.90768605124034163</v>
+      </c>
+      <c r="K29" s="105">
         <f t="shared" si="21"/>
-        <v>0.90768605124034163</v>
-      </c>
-      <c r="K29" s="106">
-        <f t="shared" si="22"/>
         <v>1.2307692307692308</v>
       </c>
     </row>
@@ -5150,15 +5151,15 @@
       <c r="B30" s="21">
         <v>1000</v>
       </c>
-      <c r="C30" s="95">
+      <c r="C30" s="94">
         <f>(C14-$C$17)/C14</f>
         <v>5.56640625E-2</v>
       </c>
-      <c r="D30" s="95">
+      <c r="D30" s="94">
         <f>(D14-$D$17)/D14</f>
         <v>0.10526315789473685</v>
       </c>
-      <c r="E30" s="95">
+      <c r="E30" s="94">
         <f>(E14-$E$17)/E14</f>
         <v>0.17777777777777778</v>
       </c>
@@ -5168,15 +5169,15 @@
       <c r="H30" s="21">
         <v>1000</v>
       </c>
-      <c r="I30" s="107">
+      <c r="I30" s="106">
         <f>C14/$C$17</f>
         <v>1.0589451913133403</v>
       </c>
-      <c r="J30" s="107">
+      <c r="J30" s="106">
         <f>D14/$D$17</f>
         <v>1.1176470588235294</v>
       </c>
-      <c r="K30" s="107">
+      <c r="K30" s="106">
         <f>E14/$E$17</f>
         <v>1.2162162162162162</v>
       </c>
@@ -5186,32 +5187,32 @@
       <c r="B31" s="3">
         <v>100</v>
       </c>
-      <c r="C31" s="95">
-        <f t="shared" ref="C31:C32" si="23">(C15-$C$17)/C15</f>
+      <c r="C31" s="94">
+        <f t="shared" ref="C31:C32" si="22">(C15-$C$17)/C15</f>
         <v>0.3102710413694722</v>
       </c>
-      <c r="D31" s="95">
-        <f t="shared" ref="D31:D32" si="24">(D15-$D$17)/D15</f>
+      <c r="D31" s="94">
+        <f t="shared" ref="D31:D32" si="23">(D15-$D$17)/D15</f>
         <v>0.6061619297826607</v>
       </c>
-      <c r="E31" s="95">
-        <f t="shared" ref="E31:E32" si="25">(E15-$E$17)/E15</f>
+      <c r="E31" s="94">
+        <f>(E15-$E$17)/E15</f>
         <v>0.7944444444444444</v>
       </c>
       <c r="G31" s="23"/>
       <c r="H31" s="3">
         <v>100</v>
       </c>
-      <c r="I31" s="107">
-        <f t="shared" ref="I31:I32" si="26">C15/$C$17</f>
+      <c r="I31" s="106">
+        <f t="shared" ref="I31:I32" si="24">C15/$C$17</f>
         <v>1.4498448810754911</v>
       </c>
-      <c r="J31" s="107">
-        <f t="shared" ref="J31:J32" si="27">D15/$D$17</f>
+      <c r="J31" s="106">
+        <f t="shared" ref="J31:J32" si="25">D15/$D$17</f>
         <v>2.5391146149181325</v>
       </c>
-      <c r="K31" s="107">
-        <f t="shared" ref="K31:K32" si="28">E15/$E$17</f>
+      <c r="K31" s="106">
+        <f t="shared" ref="K31:K32" si="26">E15/$E$17</f>
         <v>4.8648648648648649</v>
       </c>
     </row>
@@ -5220,137 +5221,137 @@
       <c r="B32" s="81">
         <v>500</v>
       </c>
-      <c r="C32" s="95">
+      <c r="C32" s="94">
+        <f t="shared" si="22"/>
+        <v>9.1165413533834588E-2</v>
+      </c>
+      <c r="D32" s="94">
         <f t="shared" si="23"/>
-        <v>9.1165413533834588E-2</v>
-      </c>
-      <c r="D32" s="95">
-        <f t="shared" si="24"/>
         <v>0.35661334373780723</v>
       </c>
-      <c r="E32" s="95">
-        <f t="shared" si="25"/>
+      <c r="E32" s="94">
+        <f t="shared" ref="E31:E32" si="27">(E16-$E$17)/E16</f>
         <v>0.72388059701492535</v>
       </c>
       <c r="G32" s="25"/>
       <c r="H32" s="81">
         <v>500</v>
       </c>
-      <c r="I32" s="107">
+      <c r="I32" s="106">
+        <f t="shared" si="24"/>
+        <v>1.1003102378490175</v>
+      </c>
+      <c r="J32" s="106">
+        <f t="shared" si="25"/>
+        <v>1.5542753183747724</v>
+      </c>
+      <c r="K32" s="106">
         <f t="shared" si="26"/>
-        <v>1.1003102378490175</v>
-      </c>
-      <c r="J32" s="107">
-        <f t="shared" si="27"/>
-        <v>1.5542753183747724</v>
-      </c>
-      <c r="K32" s="107">
-        <f t="shared" si="28"/>
         <v>3.6216216216216215</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="104" t="s">
+      <c r="A33" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="B33" s="101">
-        <v>1000</v>
-      </c>
-      <c r="C33" s="105">
+      <c r="B33" s="100">
+        <v>1000</v>
+      </c>
+      <c r="C33" s="104">
         <f>AVERAGE(C21,C24,C27,C30)</f>
         <v>0.16686212557582963</v>
       </c>
-      <c r="D33" s="105">
-        <f t="shared" ref="D33" si="29">AVERAGE(D21,D24,D27,D30)</f>
+      <c r="D33" s="104">
+        <f t="shared" ref="D33" si="28">AVERAGE(D21,D24,D27,D30)</f>
         <v>0.23671270916001977</v>
       </c>
-      <c r="E33" s="105">
+      <c r="E33" s="104">
         <f>AVERAGE(E21,E24,E27,E30)</f>
         <v>-7.4494949494949503E-2</v>
       </c>
-      <c r="G33" s="104" t="s">
+      <c r="G33" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="H33" s="101">
-        <v>1000</v>
-      </c>
-      <c r="I33" s="108">
+      <c r="H33" s="100">
+        <v>1000</v>
+      </c>
+      <c r="I33" s="107">
         <f>AVERAGE(I21,I24,I27,I30)</f>
         <v>1.2252552577674347</v>
       </c>
-      <c r="J33" s="108">
-        <f t="shared" ref="J33" si="30">AVERAGE(J21,J24,J27,J30)</f>
+      <c r="J33" s="107">
+        <f t="shared" ref="J33" si="29">AVERAGE(J21,J24,J27,J30)</f>
         <v>1.6399481532220546</v>
       </c>
-      <c r="K33" s="108">
+      <c r="K33" s="107">
         <f>AVERAGE(K21,K24,K27,K30)</f>
         <v>1.1198435277382646</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" s="104"/>
-      <c r="B34" s="102">
-        <v>100</v>
-      </c>
-      <c r="C34" s="105">
-        <f t="shared" ref="C34:E35" si="31">AVERAGE(C22,C25,C28,C31)</f>
+      <c r="A34" s="103"/>
+      <c r="B34" s="101">
+        <v>100</v>
+      </c>
+      <c r="C34" s="104">
+        <f t="shared" ref="C34:E35" si="30">AVERAGE(C22,C25,C28,C31)</f>
         <v>0.41292162836118818</v>
       </c>
-      <c r="D34" s="105">
+      <c r="D34" s="104">
+        <f t="shared" si="30"/>
+        <v>0.39057236964142694</v>
+      </c>
+      <c r="E34" s="104">
+        <f t="shared" si="30"/>
+        <v>0.61656911476296739</v>
+      </c>
+      <c r="G34" s="103"/>
+      <c r="H34" s="101">
+        <v>100</v>
+      </c>
+      <c r="I34" s="107">
+        <f t="shared" ref="I34:K35" si="31">AVERAGE(I22,I25,I28,I31)</f>
+        <v>1.8279848190889318</v>
+      </c>
+      <c r="J34" s="107">
         <f t="shared" si="31"/>
-        <v>0.39057236964142694</v>
-      </c>
-      <c r="E34" s="105">
+        <v>2.0223284841220992</v>
+      </c>
+      <c r="K34" s="107">
         <f t="shared" si="31"/>
-        <v>0.61656911476296739</v>
-      </c>
-      <c r="G34" s="104"/>
-      <c r="H34" s="102">
-        <v>100</v>
-      </c>
-      <c r="I34" s="108">
-        <f t="shared" ref="I34:K35" si="32">AVERAGE(I22,I25,I28,I31)</f>
-        <v>1.8279848190889318</v>
-      </c>
-      <c r="J34" s="108">
-        <f t="shared" si="32"/>
-        <v>2.0223284841220992</v>
-      </c>
-      <c r="K34" s="108">
-        <f t="shared" si="32"/>
         <v>3.4348396979975928</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" s="104"/>
-      <c r="B35" s="103">
+      <c r="A35" s="103"/>
+      <c r="B35" s="102">
         <v>500</v>
       </c>
-      <c r="C35" s="105">
-        <f t="shared" si="31"/>
+      <c r="C35" s="104">
+        <f t="shared" si="30"/>
         <v>-0.10737297690606165</v>
       </c>
-      <c r="D35" s="105">
+      <c r="D35" s="104">
         <f>AVERAGE(D23,D26,D29,D32)</f>
         <v>8.4282135931903965E-2</v>
       </c>
-      <c r="E35" s="105">
+      <c r="E35" s="104">
+        <f t="shared" si="30"/>
+        <v>4.5793867202449268E-2</v>
+      </c>
+      <c r="G35" s="103"/>
+      <c r="H35" s="102">
+        <v>500</v>
+      </c>
+      <c r="I35" s="107">
         <f t="shared" si="31"/>
-        <v>4.5793867202449268E-2</v>
-      </c>
-      <c r="G35" s="104"/>
-      <c r="H35" s="103">
-        <v>500</v>
-      </c>
-      <c r="I35" s="108">
-        <f t="shared" si="32"/>
         <v>0.94300505018449243</v>
       </c>
-      <c r="J35" s="108">
+      <c r="J35" s="107">
         <f>AVERAGE(J23,J26,J29,J32)</f>
         <v>1.1419166305049759</v>
       </c>
-      <c r="K35" s="108">
+      <c r="K35" s="107">
         <f>AVERAGE(K23,K26,K29,K32)</f>
         <v>1.581518765729292</v>
       </c>

</xml_diff>